<commit_message>
Change ints to size_t where applicable; Treat all warnings as errors
</commit_message>
<xml_diff>
--- a/recursivefilter.xlsx
+++ b/recursivefilter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\recursivefilter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9BAA84-EB19-4A22-8544-9DBA0FF2AEDD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A087B255-510E-45D7-9E4C-839A8D17B1BC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{678362C0-2759-4A65-8D7C-538BF80720F9}"/>
   </bookViews>
@@ -106,7 +106,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -143,13 +143,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
+      <left/>
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -164,7 +162,142 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -176,7 +309,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -200,8 +333,36 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,8 +684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FA7F144-7574-43E2-A102-27BDE7BCC9E2}">
   <dimension ref="A1:AP63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -849,7 +1010,7 @@
         <f>$B$2*D2+$B$3*K8</f>
         <v>1</v>
       </c>
-      <c r="L9" s="19">
+      <c r="L9" s="20">
         <f t="shared" ref="L9:P9" si="1">$B$2*E2+$B$3*L8</f>
         <v>0</v>
       </c>
@@ -951,11 +1112,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K10" s="20">
+      <c r="K10" s="21">
         <f>$B$2*D3+$B$3*K9</f>
         <v>3</v>
       </c>
-      <c r="L10" s="20">
+      <c r="L10" s="22">
         <f t="shared" ref="L10:P10" si="6">$B$2*E3+$B$3*L9</f>
         <v>1</v>
       </c>
@@ -1384,7 +1545,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:42" ht="10.8" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:42" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D16" s="2">
         <f>$B$2*D9+$B$3*C16</f>
         <v>1</v>
@@ -1409,67 +1571,67 @@
         <f t="shared" si="22"/>
         <v>3</v>
       </c>
-      <c r="K16" s="11">
+      <c r="K16" s="31">
         <f>K10+$B$3*$B$3*K8</f>
         <v>3</v>
       </c>
-      <c r="L16" s="11">
+      <c r="L16" s="35">
         <f t="shared" ref="L16:P16" si="23">L10+$B$3*$B$3*L8</f>
         <v>1</v>
       </c>
-      <c r="M16" s="11">
+      <c r="M16" s="30">
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
-      <c r="N16" s="11">
+      <c r="N16" s="30">
         <f t="shared" si="23"/>
         <v>2</v>
       </c>
-      <c r="O16" s="11">
+      <c r="O16" s="30">
         <f t="shared" si="23"/>
         <v>3</v>
       </c>
-      <c r="P16" s="11">
+      <c r="P16" s="30">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="R16" s="4">
+      <c r="R16" s="40">
         <f>$B$2*K16+$B$3*Q16</f>
         <v>3</v>
       </c>
-      <c r="S16" s="5">
+      <c r="S16" s="41">
         <f>$B$2*L16+$B$3*R16</f>
         <v>4</v>
       </c>
-      <c r="T16" s="4">
+      <c r="T16" s="37">
         <f>$B$2*M16+$B$3*Q16</f>
         <v>1</v>
       </c>
-      <c r="U16" s="5">
+      <c r="U16" s="34">
         <f>$B$2*N16+$B$3*T16</f>
         <v>3</v>
       </c>
-      <c r="V16" s="4">
+      <c r="V16" s="33">
         <f>$B$2*O16+$B$3*Q16</f>
         <v>3</v>
       </c>
-      <c r="W16" s="5">
+      <c r="W16" s="34">
         <f>$B$2*P16+$B$3*V16</f>
         <v>3</v>
       </c>
-      <c r="Y16" s="6">
+      <c r="Y16" s="46">
         <f>S9+$B$3*$B$3*X16+$B$3*S15</f>
         <v>1</v>
       </c>
-      <c r="Z16" s="6">
+      <c r="Z16" s="47">
         <f>U9+$B$3*$B$3*Y16+$B$3*U15</f>
         <v>2</v>
       </c>
-      <c r="AA16" s="6">
+      <c r="AA16" s="47">
         <f>W9+$B$3*$B$3*Z16+$B$3*W15</f>
         <v>3</v>
       </c>
-      <c r="AB16" s="1"/>
+      <c r="AB16" s="48"/>
       <c r="AC16" s="1"/>
       <c r="AD16" s="1" t="str">
         <f>K16 &amp; "f,"</f>
@@ -1541,67 +1703,67 @@
         <f t="shared" si="29"/>
         <v>10</v>
       </c>
-      <c r="K17" s="11">
+      <c r="K17" s="32">
         <f>K12+$B$3*$B$3*K16</f>
         <v>5</v>
       </c>
-      <c r="L17" s="11">
+      <c r="L17" s="35">
         <f t="shared" ref="L17:P17" si="30">L12+$B$3*$B$3*L16</f>
         <v>4</v>
       </c>
-      <c r="M17" s="11">
+      <c r="M17" s="30">
         <f t="shared" si="30"/>
         <v>2</v>
       </c>
-      <c r="N17" s="11">
+      <c r="N17" s="30">
         <f t="shared" si="30"/>
         <v>5</v>
       </c>
-      <c r="O17" s="11">
+      <c r="O17" s="30">
         <f t="shared" si="30"/>
         <v>4</v>
       </c>
-      <c r="P17" s="11">
+      <c r="P17" s="30">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="R17" s="4">
+      <c r="R17" s="38">
         <f t="shared" ref="R17:S17" si="31">$B$2*K17+$B$3*Q17</f>
         <v>5</v>
       </c>
-      <c r="S17" s="5">
+      <c r="S17" s="39">
         <f t="shared" si="31"/>
         <v>9</v>
       </c>
-      <c r="T17" s="4">
+      <c r="T17" s="33">
         <f t="shared" ref="T17:T18" si="32">$B$2*M17+$B$3*Q17</f>
         <v>2</v>
       </c>
-      <c r="U17" s="5">
+      <c r="U17" s="34">
         <f t="shared" ref="U17:U18" si="33">$B$2*N17+$B$3*T17</f>
         <v>7</v>
       </c>
-      <c r="V17" s="4">
+      <c r="V17" s="33">
         <f t="shared" ref="V17:V18" si="34">$B$2*O17+$B$3*Q17</f>
         <v>4</v>
       </c>
-      <c r="W17" s="5">
+      <c r="W17" s="34">
         <f t="shared" ref="W17:W18" si="35">$B$2*P17+$B$3*V17</f>
         <v>4</v>
       </c>
-      <c r="Y17" s="6">
+      <c r="Y17" s="44">
         <f>S10+$B$3*$B$3*X17+$B$3*$B$3*S15</f>
         <v>4</v>
       </c>
-      <c r="Z17" s="6">
+      <c r="Z17" s="44">
         <f>U10+$B$3*$B$3*Y17+$B$3*U15</f>
         <v>7</v>
       </c>
-      <c r="AA17" s="6">
+      <c r="AA17" s="44">
         <f>W10+$B$3*$B$3*Z17+$B$3*W15</f>
         <v>10</v>
       </c>
-      <c r="AB17" s="1"/>
+      <c r="AB17" s="45"/>
       <c r="AC17" s="1"/>
       <c r="AD17" s="1" t="str">
         <f t="shared" ref="AD17:AD18" si="36">K17 &amp; "f,"</f>
@@ -1673,67 +1835,67 @@
         <f t="shared" si="40"/>
         <v>16</v>
       </c>
-      <c r="K18" s="11">
+      <c r="K18" s="32">
         <f>K14+$B$3*$B$3*K17</f>
         <v>5</v>
       </c>
-      <c r="L18" s="11">
+      <c r="L18" s="35">
         <f t="shared" ref="L18:P18" si="41">L14+$B$3*$B$3*L17</f>
         <v>5</v>
       </c>
-      <c r="M18" s="11">
+      <c r="M18" s="30">
         <f t="shared" si="41"/>
         <v>4</v>
       </c>
-      <c r="N18" s="11">
+      <c r="N18" s="30">
         <f t="shared" si="41"/>
         <v>6</v>
       </c>
-      <c r="O18" s="11">
+      <c r="O18" s="30">
         <f t="shared" si="41"/>
         <v>6</v>
       </c>
-      <c r="P18" s="11">
+      <c r="P18" s="30">
         <f t="shared" si="41"/>
         <v>0</v>
       </c>
-      <c r="R18" s="4">
+      <c r="R18" s="33">
         <f t="shared" ref="R18:S18" si="42">$B$2*K18+$B$3*Q18</f>
         <v>5</v>
       </c>
-      <c r="S18" s="5">
+      <c r="S18" s="34">
         <f t="shared" si="42"/>
         <v>10</v>
       </c>
-      <c r="T18" s="4">
+      <c r="T18" s="33">
         <f t="shared" si="32"/>
         <v>4</v>
       </c>
-      <c r="U18" s="5">
+      <c r="U18" s="34">
         <f t="shared" si="33"/>
         <v>10</v>
       </c>
-      <c r="V18" s="4">
+      <c r="V18" s="33">
         <f t="shared" si="34"/>
         <v>6</v>
       </c>
-      <c r="W18" s="5">
+      <c r="W18" s="34">
         <f t="shared" si="35"/>
         <v>6</v>
       </c>
-      <c r="Y18" s="6">
+      <c r="Y18" s="42">
         <f>S11+$B$3*$B$3*X18+$B$3*S16</f>
         <v>7</v>
       </c>
-      <c r="Z18" s="6">
+      <c r="Z18" s="42">
         <f>U11+$B$3*$B$3*Y18+$B$3*U16</f>
         <v>13</v>
       </c>
-      <c r="AA18" s="6">
+      <c r="AA18" s="42">
         <f>W11+$B$3*$B$3*Z18+$B$3*W16</f>
         <v>16</v>
       </c>
-      <c r="AB18" s="1"/>
+      <c r="AB18" s="43"/>
       <c r="AC18" s="1"/>
       <c r="AD18" s="1" t="str">
         <f t="shared" si="36"/>
@@ -1780,7 +1942,7 @@
         <v>16f,</v>
       </c>
     </row>
-    <row r="19" spans="4:42" x14ac:dyDescent="0.2">
+    <row r="19" spans="4:42" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D19" s="2">
         <f t="shared" ref="D19:I19" si="43">$B$2*D12+$B$3*C19</f>
         <v>5</v>
@@ -1805,19 +1967,31 @@
         <f t="shared" si="43"/>
         <v>20</v>
       </c>
-      <c r="Y19" s="6">
+      <c r="K19" s="36"/>
+      <c r="L19" s="24"/>
+      <c r="M19" s="23"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="23"/>
+      <c r="P19" s="23"/>
+      <c r="R19" s="23"/>
+      <c r="S19" s="23"/>
+      <c r="T19" s="23"/>
+      <c r="U19" s="23"/>
+      <c r="V19" s="23"/>
+      <c r="W19" s="23"/>
+      <c r="Y19" s="42">
         <f>S12+$B$3*$B$3*X19+$B$3*$B$3*S16</f>
         <v>9</v>
       </c>
-      <c r="Z19" s="6">
+      <c r="Z19" s="42">
         <f>U12+$B$3*$B$3*Y19+$B$3*$B$3*U16</f>
         <v>16</v>
       </c>
-      <c r="AA19" s="6">
+      <c r="AA19" s="42">
         <f>W12+$B$3*$B$3*Z19+$B$3*$B$3*W16</f>
         <v>20</v>
       </c>
-      <c r="AB19" s="1"/>
+      <c r="AB19" s="43"/>
       <c r="AC19" s="1"/>
       <c r="AN19" s="1" t="str">
         <f t="shared" si="28"/>
@@ -1857,19 +2031,19 @@
         <f t="shared" si="44"/>
         <v>26</v>
       </c>
-      <c r="Y20" s="6">
+      <c r="Y20" s="42">
         <f>S13+$B$3*$B$3*X20+$B$3*S17</f>
         <v>10</v>
       </c>
-      <c r="Z20" s="6">
+      <c r="Z20" s="42">
         <f>U13+$B$3*$B$3*Y20+$B$3*U17</f>
         <v>20</v>
       </c>
-      <c r="AA20" s="6">
+      <c r="AA20" s="42">
         <f>W13+$B$3*$B$3*Z20+$B$3*W17</f>
         <v>26</v>
       </c>
-      <c r="AB20" s="1"/>
+      <c r="AB20" s="43"/>
       <c r="AC20" s="1"/>
       <c r="AN20" s="1" t="str">
         <f t="shared" si="28"/>
@@ -1909,43 +2083,46 @@
         <f t="shared" si="45"/>
         <v>26</v>
       </c>
-      <c r="Y21" s="6">
+      <c r="Y21" s="42">
         <f>S14+$B$3*$B$3*X21+$B$3*$B$3*S17</f>
         <v>10</v>
       </c>
-      <c r="Z21" s="6">
+      <c r="Z21" s="42">
         <f>U14+$B$3*$B$3*Y21+$B$3*$B$3*U17</f>
         <v>20</v>
       </c>
-      <c r="AA21" s="6">
+      <c r="AA21" s="42">
         <f>W14+$B$3*$B$3*Z21+$B$3*$B$3*W17</f>
         <v>26</v>
       </c>
-      <c r="AB21" s="1"/>
+      <c r="AB21" s="43"/>
       <c r="AC21" s="1"/>
     </row>
-    <row r="22" spans="4:42" x14ac:dyDescent="0.2">
-      <c r="AB22" s="1"/>
+    <row r="22" spans="4:42" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y22" s="23"/>
+      <c r="Z22" s="23"/>
+      <c r="AA22" s="23"/>
+      <c r="AB22" s="43"/>
       <c r="AC22" s="1"/>
     </row>
     <row r="23" spans="4:42" x14ac:dyDescent="0.2">
-      <c r="K23" s="2">
+      <c r="K23" s="26">
         <f>K9+$B$3*K15</f>
         <v>1</v>
       </c>
-      <c r="L23" s="2">
+      <c r="L23" s="27">
         <f t="shared" ref="L23:P23" si="46">L9+$B$3*L15</f>
         <v>0</v>
       </c>
-      <c r="M23" s="2">
+      <c r="M23" s="24">
         <f t="shared" si="46"/>
         <v>0</v>
       </c>
-      <c r="N23" s="2">
+      <c r="N23" s="23">
         <f t="shared" si="46"/>
         <v>1</v>
       </c>
-      <c r="O23" s="2">
+      <c r="O23" s="23">
         <f t="shared" si="46"/>
         <v>1</v>
       </c>
@@ -1953,23 +2130,23 @@
         <f t="shared" si="46"/>
         <v>0</v>
       </c>
-      <c r="R23" s="2">
+      <c r="R23" s="26">
         <f t="shared" ref="R23:R28" si="47">$B$2*K23+$B$3*X16</f>
         <v>1</v>
       </c>
-      <c r="S23" s="2">
+      <c r="S23" s="27">
         <f t="shared" ref="S23:S28" si="48">$B$2*L23+$B$3*R23</f>
         <v>1</v>
       </c>
-      <c r="T23" s="2">
+      <c r="T23" s="24">
         <f t="shared" ref="T23:T28" si="49">$B$2*M23+$B$3*Y16</f>
         <v>1</v>
       </c>
-      <c r="U23" s="2">
+      <c r="U23" s="23">
         <f t="shared" ref="U23:U28" si="50">$B$2*N23+$B$3*T23</f>
         <v>2</v>
       </c>
-      <c r="V23" s="2">
+      <c r="V23" s="23">
         <f t="shared" ref="V23:V28" si="51">$B$2*O23+$B$3*Z16</f>
         <v>3</v>
       </c>
@@ -1977,6 +2154,10 @@
         <f t="shared" ref="W23:W28" si="52">$B$2*P23+$B$3*V23</f>
         <v>3</v>
       </c>
+      <c r="Y23" s="23"/>
+      <c r="Z23" s="23"/>
+      <c r="AA23" s="23"/>
+      <c r="AB23" s="23"/>
       <c r="AD23" s="1" t="str">
         <f t="shared" ref="AD23:AH27" si="53">R23 &amp; "f,"</f>
         <v>1f,</v>
@@ -1999,24 +2180,24 @@
       </c>
       <c r="AI23" s="2"/>
     </row>
-    <row r="24" spans="4:42" x14ac:dyDescent="0.2">
-      <c r="K24" s="2">
+    <row r="24" spans="4:42" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K24" s="28">
         <f>K10+$B$3*$B$3*K15</f>
         <v>3</v>
       </c>
-      <c r="L24" s="2">
+      <c r="L24" s="29">
         <f t="shared" ref="L24:P24" si="54">L10+$B$3*$B$3*L15</f>
         <v>1</v>
       </c>
-      <c r="M24" s="2">
+      <c r="M24" s="24">
         <f t="shared" si="54"/>
         <v>1</v>
       </c>
-      <c r="N24" s="2">
+      <c r="N24" s="23">
         <f t="shared" si="54"/>
         <v>2</v>
       </c>
-      <c r="O24" s="2">
+      <c r="O24" s="23">
         <f t="shared" si="54"/>
         <v>3</v>
       </c>
@@ -2024,23 +2205,23 @@
         <f t="shared" si="54"/>
         <v>0</v>
       </c>
-      <c r="R24" s="2">
+      <c r="R24" s="28">
         <f t="shared" si="47"/>
         <v>3</v>
       </c>
-      <c r="S24" s="2">
+      <c r="S24" s="29">
         <f t="shared" si="48"/>
         <v>4</v>
       </c>
-      <c r="T24" s="2">
+      <c r="T24" s="24">
         <f t="shared" si="49"/>
         <v>5</v>
       </c>
-      <c r="U24" s="2">
+      <c r="U24" s="23">
         <f t="shared" si="50"/>
         <v>7</v>
       </c>
-      <c r="V24" s="2">
+      <c r="V24" s="23">
         <f t="shared" si="51"/>
         <v>10</v>
       </c>
@@ -2071,23 +2252,23 @@
       <c r="AI24" s="2"/>
     </row>
     <row r="25" spans="4:42" x14ac:dyDescent="0.2">
-      <c r="K25" s="2">
+      <c r="K25" s="25">
         <f>K11+$B$3*K16</f>
         <v>4</v>
       </c>
-      <c r="L25" s="2">
+      <c r="L25" s="25">
         <f t="shared" ref="L25:P25" si="55">L11+$B$3*L16</f>
         <v>3</v>
       </c>
-      <c r="M25" s="2">
+      <c r="M25" s="23">
         <f t="shared" si="55"/>
         <v>2</v>
       </c>
-      <c r="N25" s="2">
+      <c r="N25" s="23">
         <f t="shared" si="55"/>
         <v>4</v>
       </c>
-      <c r="O25" s="2">
+      <c r="O25" s="23">
         <f t="shared" si="55"/>
         <v>3</v>
       </c>
@@ -2095,23 +2276,23 @@
         <f t="shared" si="55"/>
         <v>0</v>
       </c>
-      <c r="R25" s="2">
+      <c r="R25" s="25">
         <f t="shared" si="47"/>
         <v>4</v>
       </c>
-      <c r="S25" s="2">
+      <c r="S25" s="25">
         <f t="shared" si="48"/>
         <v>7</v>
       </c>
-      <c r="T25" s="2">
+      <c r="T25" s="23">
         <f t="shared" si="49"/>
         <v>9</v>
       </c>
-      <c r="U25" s="2">
+      <c r="U25" s="23">
         <f t="shared" si="50"/>
         <v>13</v>
       </c>
-      <c r="V25" s="2">
+      <c r="V25" s="23">
         <f t="shared" si="51"/>
         <v>16</v>
       </c>
@@ -2142,23 +2323,23 @@
       <c r="AI25" s="2"/>
     </row>
     <row r="26" spans="4:42" x14ac:dyDescent="0.2">
-      <c r="K26" s="2">
+      <c r="K26" s="23">
         <f>K12+$B$3*$B$3*K16</f>
         <v>5</v>
       </c>
-      <c r="L26" s="2">
+      <c r="L26" s="23">
         <f t="shared" ref="L26:P26" si="56">L12+$B$3*$B$3*L16</f>
         <v>4</v>
       </c>
-      <c r="M26" s="2">
+      <c r="M26" s="23">
         <f t="shared" si="56"/>
         <v>2</v>
       </c>
-      <c r="N26" s="2">
+      <c r="N26" s="23">
         <f t="shared" si="56"/>
         <v>5</v>
       </c>
-      <c r="O26" s="2">
+      <c r="O26" s="23">
         <f t="shared" si="56"/>
         <v>4</v>
       </c>
@@ -2166,23 +2347,23 @@
         <f t="shared" si="56"/>
         <v>0</v>
       </c>
-      <c r="R26" s="2">
+      <c r="R26" s="23">
         <f t="shared" si="47"/>
         <v>5</v>
       </c>
-      <c r="S26" s="2">
+      <c r="S26" s="23">
         <f t="shared" si="48"/>
         <v>9</v>
       </c>
-      <c r="T26" s="2">
+      <c r="T26" s="23">
         <f t="shared" si="49"/>
         <v>11</v>
       </c>
-      <c r="U26" s="2">
+      <c r="U26" s="23">
         <f t="shared" si="50"/>
         <v>16</v>
       </c>
-      <c r="V26" s="2">
+      <c r="V26" s="23">
         <f t="shared" si="51"/>
         <v>20</v>
       </c>
@@ -2213,23 +2394,23 @@
       <c r="AI26" s="2"/>
     </row>
     <row r="27" spans="4:42" x14ac:dyDescent="0.2">
-      <c r="K27" s="2">
+      <c r="K27" s="23">
         <f>K13+$B$3*K17</f>
         <v>5</v>
       </c>
-      <c r="L27" s="2">
+      <c r="L27" s="23">
         <f t="shared" ref="L27:P27" si="57">L13+$B$3*L17</f>
         <v>5</v>
       </c>
-      <c r="M27" s="2">
+      <c r="M27" s="23">
         <f t="shared" si="57"/>
         <v>4</v>
       </c>
-      <c r="N27" s="2">
+      <c r="N27" s="23">
         <f t="shared" si="57"/>
         <v>6</v>
       </c>
-      <c r="O27" s="2">
+      <c r="O27" s="23">
         <f t="shared" si="57"/>
         <v>6</v>
       </c>
@@ -2237,23 +2418,23 @@
         <f t="shared" si="57"/>
         <v>0</v>
       </c>
-      <c r="R27" s="2">
+      <c r="R27" s="23">
         <f t="shared" si="47"/>
         <v>5</v>
       </c>
-      <c r="S27" s="2">
+      <c r="S27" s="23">
         <f t="shared" si="48"/>
         <v>10</v>
       </c>
-      <c r="T27" s="2">
+      <c r="T27" s="23">
         <f t="shared" si="49"/>
         <v>14</v>
       </c>
-      <c r="U27" s="2">
+      <c r="U27" s="23">
         <f t="shared" si="50"/>
         <v>20</v>
       </c>
-      <c r="V27" s="2">
+      <c r="V27" s="23">
         <f t="shared" si="51"/>
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
Adjust block and grid dims to maximize occupancy
</commit_message>
<xml_diff>
--- a/recursivefilter.xlsx
+++ b/recursivefilter.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\recursivefilter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A087B255-510E-45D7-9E4C-839A8D17B1BC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{912F5322-7D9B-40D1-A050-34FCE6E27A8F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{678362C0-2759-4A65-8D7C-538BF80720F9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tiny" sheetId="1" r:id="rId1"/>
+    <sheet name="all" sheetId="1" r:id="rId1"/>
+    <sheet name="scan" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -309,7 +310,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -363,6 +364,7 @@
     <xf numFmtId="2" fontId="1" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -685,7 +687,7 @@
   <dimension ref="A1:AP63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="W24" sqref="W24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -3997,6 +3999,250 @@
       <c r="N63" s="8"/>
       <c r="O63" s="8"/>
       <c r="P63" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD8E8E2F-052F-4240-B1DD-B8A1F81807AF}">
+  <dimension ref="B2:I10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="49"/>
+    <col min="2" max="9" width="1.44140625" style="49" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="49"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B2" s="49">
+        <v>1</v>
+      </c>
+      <c r="C2" s="49">
+        <v>1</v>
+      </c>
+      <c r="D2" s="49">
+        <v>1</v>
+      </c>
+      <c r="E2" s="49">
+        <v>1</v>
+      </c>
+      <c r="F2" s="49">
+        <v>1</v>
+      </c>
+      <c r="G2" s="49">
+        <v>1</v>
+      </c>
+      <c r="H2" s="49">
+        <v>1</v>
+      </c>
+      <c r="I2" s="49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C3" s="49">
+        <f>SUM(B2:C2)</f>
+        <v>2</v>
+      </c>
+      <c r="E3" s="49">
+        <f>SUM(D2:E2)</f>
+        <v>2</v>
+      </c>
+      <c r="G3" s="49">
+        <f>SUM(F2:G2)</f>
+        <v>2</v>
+      </c>
+      <c r="I3" s="49">
+        <f>SUM(H2:I2)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="E4" s="49">
+        <f>SUM(C3,E3)</f>
+        <v>4</v>
+      </c>
+      <c r="I4" s="49">
+        <f>SUM(G3,I3)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B5" s="49">
+        <f>B2</f>
+        <v>1</v>
+      </c>
+      <c r="C5" s="49">
+        <f>C3</f>
+        <v>2</v>
+      </c>
+      <c r="D5" s="49">
+        <f>D2</f>
+        <v>1</v>
+      </c>
+      <c r="E5" s="49">
+        <f>E4</f>
+        <v>4</v>
+      </c>
+      <c r="F5" s="49">
+        <f>F2</f>
+        <v>1</v>
+      </c>
+      <c r="G5" s="49">
+        <f>G3</f>
+        <v>2</v>
+      </c>
+      <c r="H5" s="49">
+        <f>H2</f>
+        <v>1</v>
+      </c>
+      <c r="I5" s="49">
+        <f>SUM(E4,I4)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B7" s="49">
+        <f t="shared" ref="B7:H7" si="0">B5</f>
+        <v>1</v>
+      </c>
+      <c r="C7" s="49">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D7" s="49">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E7" s="49">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F7" s="49">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G7" s="49">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H7" s="49">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I7" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B8" s="49">
+        <f>B7</f>
+        <v>1</v>
+      </c>
+      <c r="C8" s="49">
+        <f>C7</f>
+        <v>2</v>
+      </c>
+      <c r="D8" s="49">
+        <f>D7</f>
+        <v>1</v>
+      </c>
+      <c r="E8" s="49">
+        <f>I7</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="49">
+        <f>F7</f>
+        <v>1</v>
+      </c>
+      <c r="G8" s="49">
+        <f>G7</f>
+        <v>2</v>
+      </c>
+      <c r="H8" s="49">
+        <f>H7</f>
+        <v>1</v>
+      </c>
+      <c r="I8" s="49">
+        <f>SUM(E7, I7)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B9" s="49">
+        <f>B8</f>
+        <v>1</v>
+      </c>
+      <c r="C9" s="49">
+        <f>E8</f>
+        <v>0</v>
+      </c>
+      <c r="D9" s="49">
+        <f>D8</f>
+        <v>1</v>
+      </c>
+      <c r="E9" s="49">
+        <f>SUM(C8, E8)</f>
+        <v>2</v>
+      </c>
+      <c r="F9" s="49">
+        <f>F8</f>
+        <v>1</v>
+      </c>
+      <c r="G9" s="49">
+        <f>I8</f>
+        <v>4</v>
+      </c>
+      <c r="H9" s="49">
+        <f>H8</f>
+        <v>1</v>
+      </c>
+      <c r="I9" s="49">
+        <f>SUM(G8, I8)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B10" s="49">
+        <f>C9</f>
+        <v>0</v>
+      </c>
+      <c r="C10" s="49">
+        <f>SUM(B9, C9)</f>
+        <v>1</v>
+      </c>
+      <c r="D10" s="49">
+        <f>E9</f>
+        <v>2</v>
+      </c>
+      <c r="E10" s="49">
+        <f>SUM(D9, E9)</f>
+        <v>3</v>
+      </c>
+      <c r="F10" s="49">
+        <f>G9</f>
+        <v>4</v>
+      </c>
+      <c r="G10" s="49">
+        <f>SUM(F9, G9)</f>
+        <v>5</v>
+      </c>
+      <c r="H10" s="49">
+        <f>I9</f>
+        <v>6</v>
+      </c>
+      <c r="I10" s="49">
+        <f>SUM(H9, I9)</f>
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4245,21 +4491,21 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4283,14 +4529,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCCBCDE3-ADC9-411E-A5F5-6F7285261F5D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{32695E15-2B13-4DDA-A339-3037F2566A9D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -4306,4 +4544,12 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCCBCDE3-ADC9-411E-A5F5-6F7285261F5D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fill final sum table as col-major; Add transpose with cuBLAS
</commit_message>
<xml_diff>
--- a/recursivefilter.xlsx
+++ b/recursivefilter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\recursivefilter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD3521BE-5613-48FB-A2B9-54FDAFCE7228}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D7C97ED-3255-437C-AA3B-8D5A3DE04291}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{678362C0-2759-4A65-8D7C-538BF80720F9}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="1">
   <si>
     <t>-</t>
   </si>
@@ -69,16 +69,14 @@
       <charset val="238"/>
     </font>
     <font>
-      <b/>
       <sz val="8"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial Narrow"/>
       <family val="2"/>
       <charset val="238"/>
     </font>
     <font>
+      <b/>
       <sz val="8"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial Narrow"/>
       <family val="2"/>
       <charset val="238"/>
@@ -477,8 +475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FA7F144-7574-43E2-A102-27BDE7BCC9E2}">
   <dimension ref="A1:AP40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="X24" sqref="X24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W10" sqref="W10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -2127,11 +2125,11 @@
       <c r="Z25" s="13">
         <v>2</v>
       </c>
-      <c r="AA25" s="6">
+      <c r="AA25" s="17">
         <f>U16+POWER($B$3,Z25)*U20+POWER($B$3,4)*0</f>
         <v>12.775446879245226</v>
       </c>
-      <c r="AB25" s="18">
+      <c r="AB25" s="17">
         <f>V16+POWER($B$3,$Z25)*V23+POWER($B$3,4)*AA25</f>
         <v>5.7250492338663506</v>
       </c>
@@ -2231,11 +2229,11 @@
       <c r="Z26" s="13">
         <v>3</v>
       </c>
-      <c r="AA26" s="6">
+      <c r="AA26" s="17">
         <f>U17+POWER($B$3,Z26)*U20+POWER($B$3,4)*0</f>
         <v>12.933298630183838</v>
       </c>
-      <c r="AB26" s="18">
+      <c r="AB26" s="17">
         <f>V17+POWER($B$3,$Z26)*V23+POWER($B$3,4)*AA26</f>
         <v>6.6241036306834085</v>
       </c>
@@ -2335,11 +2333,11 @@
       <c r="Z27" s="13">
         <v>4</v>
       </c>
-      <c r="AA27" s="17">
+      <c r="AA27" s="18">
         <f>U18+POWER($B$3,Z27)*U20+POWER($B$3,4)*0</f>
         <v>13.019485686196322</v>
       </c>
-      <c r="AB27" s="17">
+      <c r="AB27" s="18">
         <f>V18+POWER($B$3,$Z27)*V23+POWER($B$3,4)*AA27</f>
         <v>7.1149873313455236</v>
       </c>

</xml_diff>

<commit_message>
Merge transposing final sum table into step5
</commit_message>
<xml_diff>
--- a/recursivefilter.xlsx
+++ b/recursivefilter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\recursivefilter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D7C97ED-3255-437C-AA3B-8D5A3DE04291}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B315E042-20F6-43BF-880B-3CBC81DCDEBF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{678362C0-2759-4A65-8D7C-538BF80720F9}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="1">
   <si>
     <t>-</t>
   </si>
@@ -476,7 +476,7 @@
   <dimension ref="A1:AP40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W10" sqref="W10"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -529,16 +529,16 @@
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.2">
       <c r="B2" s="12">
-        <v>1.7230000000000001</v>
+        <v>1</v>
       </c>
       <c r="D2" s="13">
         <v>1</v>
       </c>
       <c r="E2" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -588,10 +588,10 @@
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.2">
       <c r="B3" s="12">
-        <v>0.54600000000000004</v>
+        <v>1</v>
       </c>
       <c r="D3" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3" s="13">
         <v>1</v>
@@ -603,7 +603,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I3" s="13">
         <v>0</v>
@@ -650,16 +650,16 @@
         <v>1</v>
       </c>
       <c r="E4" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F4" s="13">
         <v>1</v>
       </c>
       <c r="G4" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H4" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4" s="13">
         <v>0</v>
@@ -712,7 +712,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" s="13">
         <v>1</v>
@@ -765,19 +765,19 @@
         <v>0.54600000000000004</v>
       </c>
       <c r="D6" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" s="13">
         <v>1</v>
       </c>
       <c r="F6" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G6" s="13">
         <v>1</v>
       </c>
       <c r="H6" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I6" s="13">
         <v>0</v>
@@ -821,19 +821,19 @@
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D7" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I7" s="13">
         <v>0</v>
@@ -880,19 +880,19 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="D8" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8" s="13">
         <v>0</v>
@@ -918,19 +918,19 @@
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D9" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H9" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I9" s="13">
         <v>0</v>
@@ -956,688 +956,688 @@
     </row>
     <row r="11" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D11" s="2">
-        <f>$B$2*D2+$B$3*D10</f>
-        <v>1.7230000000000001</v>
+        <f t="shared" ref="D11:D18" si="0">$B$2*D2+$B$3*D10</f>
+        <v>1</v>
       </c>
       <c r="E11" s="2">
-        <f t="shared" ref="E11:I11" si="0">$B$2*E2+$B$3*E10</f>
-        <v>1.7230000000000001</v>
+        <f t="shared" ref="E11:I11" si="1">$B$2*E2+$B$3*E10</f>
+        <v>0</v>
       </c>
       <c r="F11" s="2">
-        <f t="shared" si="0"/>
-        <v>1.7230000000000001</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="G11" s="2">
-        <f t="shared" si="0"/>
-        <v>1.7230000000000001</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="H11" s="2">
-        <f t="shared" si="0"/>
-        <v>1.7230000000000001</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="I11" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K11" s="8">
-        <f>$B$2*D2</f>
-        <v>1.7230000000000001</v>
+        <f t="shared" ref="K11:P11" si="2">$B$2*D2</f>
+        <v>1</v>
       </c>
       <c r="L11" s="8">
-        <f>$B$2*E2</f>
-        <v>1.7230000000000001</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="M11" s="8">
-        <f>$B$2*F2</f>
-        <v>1.7230000000000001</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="N11" s="8">
-        <f>$B$2*G2</f>
-        <v>1.7230000000000001</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="O11" s="8">
-        <f>$B$2*H2</f>
-        <v>1.7230000000000001</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="P11" s="8">
-        <f>$B$2*I2</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R11" s="3">
         <f>$B$2*K11</f>
-        <v>2.9687290000000002</v>
+        <v>1</v>
       </c>
       <c r="S11" s="3">
-        <f t="shared" ref="S11:U11" si="1">$B$2*L11+$B$3*R11</f>
-        <v>4.5896550340000006</v>
+        <f t="shared" ref="S11:U11" si="3">$B$2*L11+$B$3*R11</f>
+        <v>1</v>
       </c>
       <c r="T11" s="3">
-        <f t="shared" si="1"/>
-        <v>5.4746806485640001</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="U11" s="11">
-        <f t="shared" si="1"/>
-        <v>5.9579046341159447</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="V11" s="3">
         <f>$B$2*O11</f>
-        <v>2.9687290000000002</v>
+        <v>1</v>
       </c>
       <c r="AD11" s="1" t="str">
         <f>K14 &amp; "f,"</f>
-        <v>3.457866879928f,</v>
+        <v>5f,</v>
       </c>
       <c r="AE11" s="1" t="str">
         <f>L14 &amp; "f,"</f>
-        <v>3.457866879928f,</v>
+        <v>4f,</v>
       </c>
       <c r="AF11" s="1" t="str">
         <f>M14 &amp; "f,"</f>
-        <v>3.457866879928f,</v>
+        <v>2f,</v>
       </c>
       <c r="AG11" s="1" t="str">
         <f>N14 &amp; "f,"</f>
-        <v>3.457866879928f,</v>
+        <v>5f,</v>
       </c>
       <c r="AH11" s="1" t="str">
         <f>O14 &amp; "f,"</f>
-        <v>3.457866879928f,</v>
+        <v>4f,</v>
       </c>
       <c r="AJ11" s="1" t="str">
         <f>U11 &amp; "f,"</f>
-        <v>5.95790463411594f,</v>
+        <v>2f,</v>
       </c>
       <c r="AK11" s="1" t="str">
         <f>V11 &amp; "f,"</f>
-        <v>2.968729f,</v>
+        <v>1f,</v>
       </c>
     </row>
     <row r="12" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D12" s="2">
-        <f>$B$2*D3+$B$3*D11</f>
-        <v>2.6637580000000001</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="E12" s="2">
-        <f>$B$2*E3+$B$3*E11</f>
-        <v>2.6637580000000001</v>
+        <f t="shared" ref="E12:I16" si="4">$B$2*E3+$B$3*E11</f>
+        <v>1</v>
       </c>
       <c r="F12" s="2">
-        <f>$B$2*F3+$B$3*F11</f>
-        <v>2.6637580000000001</v>
+        <f t="shared" si="4"/>
+        <v>1</v>
       </c>
       <c r="G12" s="2">
-        <f>$B$2*G3+$B$3*G11</f>
-        <v>2.6637580000000001</v>
+        <f t="shared" si="4"/>
+        <v>2</v>
       </c>
       <c r="H12" s="2">
-        <f>$B$2*H3+$B$3*H11</f>
-        <v>2.6637580000000001</v>
+        <f t="shared" si="4"/>
+        <v>3</v>
       </c>
       <c r="I12" s="2">
-        <f>$B$2*I3+$B$3*I11</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K12" s="8">
-        <f>$B$2*D3+$B$3*K11</f>
-        <v>2.6637580000000001</v>
+        <f t="shared" ref="K12:P14" si="5">$B$2*D3+$B$3*K11</f>
+        <v>3</v>
       </c>
       <c r="L12" s="8">
-        <f>$B$2*E3+$B$3*L11</f>
-        <v>2.6637580000000001</v>
+        <f t="shared" si="5"/>
+        <v>1</v>
       </c>
       <c r="M12" s="8">
-        <f>$B$2*F3+$B$3*M11</f>
-        <v>2.6637580000000001</v>
+        <f t="shared" si="5"/>
+        <v>1</v>
       </c>
       <c r="N12" s="8">
-        <f>$B$2*G3+$B$3*N11</f>
-        <v>2.6637580000000001</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="O12" s="8">
-        <f>$B$2*H3+$B$3*O11</f>
-        <v>2.6637580000000001</v>
+        <f t="shared" si="5"/>
+        <v>3</v>
       </c>
       <c r="P12" s="8">
-        <f>$B$2*I3+$B$3*P11</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="R12" s="3">
-        <f t="shared" ref="R12:R16" si="2">$B$2*K12</f>
-        <v>4.5896550340000006</v>
+        <f t="shared" ref="R12:R16" si="6">$B$2*K12</f>
+        <v>3</v>
       </c>
       <c r="S12" s="3">
-        <f t="shared" ref="S12:S16" si="3">$B$2*L12+$B$3*R12</f>
-        <v>7.095606682564001</v>
+        <f t="shared" ref="S12:S16" si="7">$B$2*L12+$B$3*R12</f>
+        <v>4</v>
       </c>
       <c r="T12" s="3">
-        <f t="shared" ref="T12:T16" si="4">$B$2*M12+$B$3*S12</f>
-        <v>8.4638562826799451</v>
+        <f t="shared" ref="T12:T16" si="8">$B$2*M12+$B$3*S12</f>
+        <v>5</v>
       </c>
       <c r="U12" s="11">
-        <f t="shared" ref="U12:U16" si="5">$B$2*N12+$B$3*T12</f>
-        <v>9.210920564343251</v>
+        <f t="shared" ref="U12:U16" si="9">$B$2*N12+$B$3*T12</f>
+        <v>7</v>
       </c>
       <c r="V12" s="3">
-        <f t="shared" ref="V12:V16" si="6">$B$2*O12</f>
-        <v>4.5896550340000006</v>
+        <f t="shared" ref="V12:V16" si="10">$B$2*O12</f>
+        <v>3</v>
       </c>
       <c r="AD12" s="1" t="str">
         <f>K15 &amp; "f,"</f>
-        <v>1.723f,</v>
+        <v>0f,</v>
       </c>
       <c r="AE12" s="1" t="str">
-        <f t="shared" ref="AE12:AH12" si="7">L15 &amp; "f,"</f>
-        <v>1.723f,</v>
+        <f t="shared" ref="AE12:AH12" si="11">L15 &amp; "f,"</f>
+        <v>1f,</v>
       </c>
       <c r="AF12" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>1.723f,</v>
+        <f t="shared" si="11"/>
+        <v>2f,</v>
       </c>
       <c r="AG12" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>1.723f,</v>
+        <f t="shared" si="11"/>
+        <v>1f,</v>
       </c>
       <c r="AH12" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>1.723f,</v>
+        <f t="shared" si="11"/>
+        <v>2f,</v>
       </c>
       <c r="AJ12" s="1" t="str">
-        <f t="shared" ref="AJ12:AJ15" si="8">U12 &amp; "f,"</f>
-        <v>9.21092056434325f,</v>
+        <f t="shared" ref="AJ12:AJ15" si="12">U12 &amp; "f,"</f>
+        <v>7f,</v>
       </c>
       <c r="AK12" s="1" t="str">
-        <f t="shared" ref="AK12:AK15" si="9">V12 &amp; "f,"</f>
-        <v>4.589655034f,</v>
+        <f t="shared" ref="AK12:AK15" si="13">V12 &amp; "f,"</f>
+        <v>3f,</v>
       </c>
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D13" s="2">
-        <f>$B$2*D4+$B$3*D12</f>
-        <v>3.1774118680000001</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="E13" s="2">
-        <f>$B$2*E4+$B$3*E12</f>
-        <v>3.1774118680000001</v>
+        <f t="shared" si="4"/>
+        <v>3</v>
       </c>
       <c r="F13" s="2">
-        <f>$B$2*F4+$B$3*F12</f>
-        <v>3.1774118680000001</v>
+        <f t="shared" si="4"/>
+        <v>2</v>
       </c>
       <c r="G13" s="2">
-        <f>$B$2*G4+$B$3*G12</f>
-        <v>3.1774118680000001</v>
+        <f t="shared" si="4"/>
+        <v>4</v>
       </c>
       <c r="H13" s="2">
-        <f>$B$2*H4+$B$3*H12</f>
-        <v>3.1774118680000001</v>
+        <f t="shared" si="4"/>
+        <v>3</v>
       </c>
       <c r="I13" s="2">
-        <f>$B$2*I4+$B$3*I12</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K13" s="8">
-        <f>$B$2*D4+$B$3*K12</f>
-        <v>3.1774118680000001</v>
+        <f t="shared" si="5"/>
+        <v>4</v>
       </c>
       <c r="L13" s="8">
-        <f>$B$2*E4+$B$3*L12</f>
-        <v>3.1774118680000001</v>
+        <f t="shared" si="5"/>
+        <v>3</v>
       </c>
       <c r="M13" s="8">
-        <f>$B$2*F4+$B$3*M12</f>
-        <v>3.1774118680000001</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="N13" s="8">
-        <f>$B$2*G4+$B$3*N12</f>
-        <v>3.1774118680000001</v>
+        <f t="shared" si="5"/>
+        <v>4</v>
       </c>
       <c r="O13" s="8">
-        <f>$B$2*H4+$B$3*O12</f>
-        <v>3.1774118680000001</v>
+        <f t="shared" si="5"/>
+        <v>3</v>
       </c>
       <c r="P13" s="8">
-        <f>$B$2*I4+$B$3*P12</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="R13" s="3">
-        <f t="shared" si="2"/>
-        <v>5.4746806485640001</v>
+        <f t="shared" si="6"/>
+        <v>4</v>
       </c>
       <c r="S13" s="3">
-        <f t="shared" si="3"/>
-        <v>8.4638562826799451</v>
+        <f t="shared" si="7"/>
+        <v>7</v>
       </c>
       <c r="T13" s="3">
-        <f t="shared" si="4"/>
-        <v>10.095946178907251</v>
+        <f t="shared" si="8"/>
+        <v>9</v>
       </c>
       <c r="U13" s="11">
-        <f t="shared" si="5"/>
-        <v>10.98706726224736</v>
+        <f t="shared" si="9"/>
+        <v>13</v>
       </c>
       <c r="V13" s="3">
-        <f t="shared" si="6"/>
-        <v>5.4746806485640001</v>
+        <f t="shared" si="10"/>
+        <v>3</v>
       </c>
       <c r="AJ13" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>10.9870672622474f,</v>
+        <f t="shared" si="12"/>
+        <v>13f,</v>
       </c>
       <c r="AK13" s="1" t="str">
-        <f t="shared" si="9"/>
-        <v>5.474680648564f,</v>
+        <f t="shared" si="13"/>
+        <v>3f,</v>
       </c>
     </row>
     <row r="14" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D14" s="2">
-        <f>$B$2*D5+$B$3*D13</f>
-        <v>3.4578668799280003</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="E14" s="2">
-        <f>$B$2*E5+$B$3*E13</f>
-        <v>3.4578668799280003</v>
+        <f t="shared" si="4"/>
+        <v>4</v>
       </c>
       <c r="F14" s="2">
-        <f>$B$2*F5+$B$3*F13</f>
-        <v>3.4578668799280003</v>
+        <f t="shared" si="4"/>
+        <v>2</v>
       </c>
       <c r="G14" s="2">
-        <f>$B$2*G5+$B$3*G13</f>
-        <v>3.4578668799280003</v>
+        <f t="shared" si="4"/>
+        <v>5</v>
       </c>
       <c r="H14" s="2">
-        <f>$B$2*H5+$B$3*H13</f>
-        <v>3.4578668799280003</v>
+        <f t="shared" si="4"/>
+        <v>4</v>
       </c>
       <c r="I14" s="2">
-        <f>$B$2*I5+$B$3*I13</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K14" s="9">
-        <f>$B$2*D5+$B$3*K13</f>
-        <v>3.4578668799280003</v>
+        <f t="shared" si="5"/>
+        <v>5</v>
       </c>
       <c r="L14" s="9">
-        <f>$B$2*E5+$B$3*L13</f>
-        <v>3.4578668799280003</v>
+        <f t="shared" si="5"/>
+        <v>4</v>
       </c>
       <c r="M14" s="9">
-        <f>$B$2*F5+$B$3*M13</f>
-        <v>3.4578668799280003</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="N14" s="9">
-        <f>$B$2*G5+$B$3*N13</f>
-        <v>3.4578668799280003</v>
+        <f t="shared" si="5"/>
+        <v>5</v>
       </c>
       <c r="O14" s="9">
-        <f>$B$2*H5+$B$3*O13</f>
-        <v>3.4578668799280003</v>
+        <f t="shared" si="5"/>
+        <v>4</v>
       </c>
       <c r="P14" s="9">
-        <f>$B$2*I5+$B$3*P13</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="R14" s="3">
-        <f t="shared" si="2"/>
-        <v>5.9579046341159447</v>
+        <f t="shared" si="6"/>
+        <v>5</v>
       </c>
       <c r="S14" s="3">
-        <f t="shared" si="3"/>
-        <v>9.210920564343251</v>
+        <f t="shared" si="7"/>
+        <v>9</v>
       </c>
       <c r="T14" s="3">
-        <f t="shared" si="4"/>
-        <v>10.987067262247361</v>
+        <f t="shared" si="8"/>
+        <v>11</v>
       </c>
       <c r="U14" s="11">
-        <f t="shared" si="5"/>
-        <v>11.956843359303004</v>
+        <f t="shared" si="9"/>
+        <v>16</v>
       </c>
       <c r="V14" s="3">
-        <f t="shared" si="6"/>
-        <v>5.9579046341159447</v>
+        <f t="shared" si="10"/>
+        <v>4</v>
       </c>
       <c r="AJ14" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>11.956843359303f,</v>
+        <f t="shared" si="12"/>
+        <v>16f,</v>
       </c>
       <c r="AK14" s="1" t="str">
-        <f t="shared" si="9"/>
-        <v>5.95790463411594f,</v>
+        <f t="shared" si="13"/>
+        <v>4f,</v>
       </c>
     </row>
     <row r="15" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D15" s="2">
-        <f>$B$2*D6+$B$3*D14</f>
-        <v>3.6109953164406887</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="E15" s="2">
-        <f>$B$2*E6+$B$3*E14</f>
-        <v>3.6109953164406887</v>
+        <f t="shared" si="4"/>
+        <v>5</v>
       </c>
       <c r="F15" s="2">
-        <f>$B$2*F6+$B$3*F14</f>
-        <v>3.6109953164406887</v>
+        <f t="shared" si="4"/>
+        <v>4</v>
       </c>
       <c r="G15" s="2">
-        <f>$B$2*G6+$B$3*G14</f>
-        <v>3.6109953164406887</v>
+        <f t="shared" si="4"/>
+        <v>6</v>
       </c>
       <c r="H15" s="2">
-        <f>$B$2*H6+$B$3*H14</f>
-        <v>3.6109953164406887</v>
+        <f t="shared" si="4"/>
+        <v>6</v>
       </c>
       <c r="I15" s="2">
-        <f>$B$2*I6+$B$3*I14</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K15" s="8">
-        <f>$B$2*D6</f>
-        <v>1.7230000000000001</v>
+        <f t="shared" ref="K15:P15" si="14">$B$2*D6</f>
+        <v>0</v>
       </c>
       <c r="L15" s="8">
-        <f>$B$2*E6</f>
-        <v>1.7230000000000001</v>
+        <f t="shared" si="14"/>
+        <v>1</v>
       </c>
       <c r="M15" s="8">
-        <f>$B$2*F6</f>
-        <v>1.7230000000000001</v>
+        <f t="shared" si="14"/>
+        <v>2</v>
       </c>
       <c r="N15" s="8">
-        <f>$B$2*G6</f>
-        <v>1.7230000000000001</v>
+        <f t="shared" si="14"/>
+        <v>1</v>
       </c>
       <c r="O15" s="8">
-        <f>$B$2*H6</f>
-        <v>1.7230000000000001</v>
+        <f t="shared" si="14"/>
+        <v>2</v>
       </c>
       <c r="P15" s="8">
-        <f>$B$2*I6</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="R15" s="3">
-        <f t="shared" si="2"/>
-        <v>2.9687290000000002</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="S15" s="3">
-        <f t="shared" si="3"/>
-        <v>4.5896550340000006</v>
+        <f t="shared" si="7"/>
+        <v>1</v>
       </c>
       <c r="T15" s="3">
-        <f t="shared" si="4"/>
-        <v>5.4746806485640001</v>
+        <f t="shared" si="8"/>
+        <v>3</v>
       </c>
       <c r="U15" s="11">
-        <f t="shared" si="5"/>
-        <v>5.9579046341159447</v>
+        <f t="shared" si="9"/>
+        <v>4</v>
       </c>
       <c r="V15" s="3">
-        <f t="shared" si="6"/>
-        <v>2.9687290000000002</v>
+        <f t="shared" si="10"/>
+        <v>2</v>
       </c>
       <c r="AJ15" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>5.95790463411594f,</v>
+        <f t="shared" si="12"/>
+        <v>4f,</v>
       </c>
       <c r="AK15" s="1" t="str">
-        <f t="shared" si="9"/>
-        <v>2.968729f,</v>
+        <f t="shared" si="13"/>
+        <v>2f,</v>
       </c>
     </row>
     <row r="16" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D16" s="2">
-        <f>$B$2*D7+$B$3*D15</f>
-        <v>3.6946034427766161</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="E16" s="2">
-        <f>$B$2*E7+$B$3*E15</f>
-        <v>3.6946034427766161</v>
+        <f t="shared" si="4"/>
+        <v>5</v>
       </c>
       <c r="F16" s="2">
-        <f>$B$2*F7+$B$3*F15</f>
-        <v>3.6946034427766161</v>
+        <f t="shared" si="4"/>
+        <v>4</v>
       </c>
       <c r="G16" s="2">
-        <f>$B$2*G7+$B$3*G15</f>
-        <v>3.6946034427766161</v>
+        <f t="shared" si="4"/>
+        <v>6</v>
       </c>
       <c r="H16" s="2">
-        <f>$B$2*H7+$B$3*H15</f>
-        <v>3.6946034427766161</v>
+        <f t="shared" si="4"/>
+        <v>6</v>
       </c>
       <c r="I16" s="2">
-        <f>$B$2*I7+$B$3*I15</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K16" s="8">
-        <f>$B$2*D7+$B$3*K15</f>
-        <v>2.6637580000000001</v>
+        <f t="shared" ref="K16:P18" si="15">$B$2*D7+$B$3*K15</f>
+        <v>0</v>
       </c>
       <c r="L16" s="8">
-        <f>$B$2*E7+$B$3*L15</f>
-        <v>2.6637580000000001</v>
+        <f t="shared" si="15"/>
+        <v>1</v>
       </c>
       <c r="M16" s="8">
-        <f>$B$2*F7+$B$3*M15</f>
-        <v>2.6637580000000001</v>
+        <f t="shared" si="15"/>
+        <v>2</v>
       </c>
       <c r="N16" s="8">
-        <f>$B$2*G7+$B$3*N15</f>
-        <v>2.6637580000000001</v>
+        <f t="shared" si="15"/>
+        <v>1</v>
       </c>
       <c r="O16" s="8">
-        <f>$B$2*H7+$B$3*O15</f>
-        <v>2.6637580000000001</v>
+        <f t="shared" si="15"/>
+        <v>2</v>
       </c>
       <c r="P16" s="8">
-        <f>$B$2*I7+$B$3*P15</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="R16" s="3">
-        <f t="shared" si="2"/>
-        <v>4.5896550340000006</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="S16" s="3">
-        <f t="shared" si="3"/>
-        <v>7.095606682564001</v>
+        <f t="shared" si="7"/>
+        <v>1</v>
       </c>
       <c r="T16" s="3">
-        <f t="shared" si="4"/>
-        <v>8.4638562826799451</v>
+        <f t="shared" si="8"/>
+        <v>3</v>
       </c>
       <c r="U16" s="11">
-        <f t="shared" si="5"/>
-        <v>9.210920564343251</v>
+        <f t="shared" si="9"/>
+        <v>4</v>
       </c>
       <c r="V16" s="3">
-        <f t="shared" si="6"/>
-        <v>4.5896550340000006</v>
+        <f t="shared" si="10"/>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="4:42" x14ac:dyDescent="0.2">
       <c r="D17" s="2">
-        <f>$B$2*D8+$B$3*D16</f>
-        <v>3.7402534797560323</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="E17" s="2">
-        <f t="shared" ref="E17:I17" si="10">$B$2*E8+$B$3*E16</f>
-        <v>3.7402534797560323</v>
+        <f t="shared" ref="E17:I17" si="16">$B$2*E8+$B$3*E16</f>
+        <v>5</v>
       </c>
       <c r="F17" s="2">
-        <f t="shared" si="10"/>
-        <v>3.7402534797560323</v>
+        <f t="shared" si="16"/>
+        <v>4</v>
       </c>
       <c r="G17" s="2">
-        <f t="shared" si="10"/>
-        <v>3.7402534797560323</v>
+        <f t="shared" si="16"/>
+        <v>6</v>
       </c>
       <c r="H17" s="2">
-        <f t="shared" si="10"/>
-        <v>3.7402534797560323</v>
+        <f t="shared" si="16"/>
+        <v>6</v>
       </c>
       <c r="I17" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="K17" s="8">
-        <f>$B$2*D8+$B$3*K16</f>
-        <v>3.1774118680000001</v>
+        <f t="shared" si="15"/>
+        <v>0</v>
       </c>
       <c r="L17" s="8">
-        <f>$B$2*E8+$B$3*L16</f>
-        <v>3.1774118680000001</v>
+        <f t="shared" si="15"/>
+        <v>1</v>
       </c>
       <c r="M17" s="8">
-        <f>$B$2*F8+$B$3*M16</f>
-        <v>3.1774118680000001</v>
+        <f t="shared" si="15"/>
+        <v>2</v>
       </c>
       <c r="N17" s="8">
-        <f>$B$2*G8+$B$3*N16</f>
-        <v>3.1774118680000001</v>
+        <f t="shared" si="15"/>
+        <v>1</v>
       </c>
       <c r="O17" s="8">
-        <f>$B$2*H8+$B$3*O16</f>
-        <v>3.1774118680000001</v>
+        <f t="shared" si="15"/>
+        <v>2</v>
       </c>
       <c r="P17" s="8">
-        <f>$B$2*I8+$B$3*P16</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="R17" s="3">
-        <f t="shared" ref="R17:R18" si="11">$B$2*K17</f>
-        <v>5.4746806485640001</v>
+        <f t="shared" ref="R17:R18" si="17">$B$2*K17</f>
+        <v>0</v>
       </c>
       <c r="S17" s="3">
-        <f t="shared" ref="S17:S18" si="12">$B$2*L17+$B$3*R17</f>
-        <v>8.4638562826799451</v>
+        <f t="shared" ref="S17:S18" si="18">$B$2*L17+$B$3*R17</f>
+        <v>1</v>
       </c>
       <c r="T17" s="3">
-        <f t="shared" ref="T17:T18" si="13">$B$2*M17+$B$3*S17</f>
-        <v>10.095946178907251</v>
+        <f t="shared" ref="T17:T18" si="19">$B$2*M17+$B$3*S17</f>
+        <v>3</v>
       </c>
       <c r="U17" s="11">
-        <f t="shared" ref="U17:U18" si="14">$B$2*N17+$B$3*T17</f>
-        <v>10.98706726224736</v>
+        <f t="shared" ref="U17:U18" si="20">$B$2*N17+$B$3*T17</f>
+        <v>4</v>
       </c>
       <c r="V17" s="3">
-        <f t="shared" ref="V17:V18" si="15">$B$2*O17</f>
-        <v>5.4746806485640001</v>
+        <f t="shared" ref="V17:V18" si="21">$B$2*O17</f>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="4:42" x14ac:dyDescent="0.2">
       <c r="D18" s="2">
-        <f>$B$2*D9+$B$3*D17</f>
-        <v>3.7651783999467936</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="E18" s="2">
-        <f t="shared" ref="E18:I18" si="16">$B$2*E9+$B$3*E17</f>
-        <v>3.7651783999467936</v>
+        <f t="shared" ref="E18:I18" si="22">$B$2*E9+$B$3*E17</f>
+        <v>5</v>
       </c>
       <c r="F18" s="2">
-        <f t="shared" si="16"/>
-        <v>3.7651783999467936</v>
+        <f t="shared" si="22"/>
+        <v>4</v>
       </c>
       <c r="G18" s="2">
-        <f t="shared" si="16"/>
-        <v>3.7651783999467936</v>
+        <f t="shared" si="22"/>
+        <v>6</v>
       </c>
       <c r="H18" s="2">
-        <f t="shared" si="16"/>
-        <v>3.7651783999467936</v>
+        <f t="shared" si="22"/>
+        <v>6</v>
       </c>
       <c r="I18" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="K18" s="9">
-        <f>$B$2*D9+$B$3*K17</f>
-        <v>3.4578668799280003</v>
+        <f t="shared" si="15"/>
+        <v>0</v>
       </c>
       <c r="L18" s="9">
-        <f>$B$2*E9+$B$3*L17</f>
-        <v>3.4578668799280003</v>
+        <f t="shared" si="15"/>
+        <v>1</v>
       </c>
       <c r="M18" s="9">
-        <f>$B$2*F9+$B$3*M17</f>
-        <v>3.4578668799280003</v>
+        <f t="shared" si="15"/>
+        <v>2</v>
       </c>
       <c r="N18" s="9">
-        <f>$B$2*G9+$B$3*N17</f>
-        <v>3.4578668799280003</v>
+        <f t="shared" si="15"/>
+        <v>1</v>
       </c>
       <c r="O18" s="9">
-        <f>$B$2*H9+$B$3*O17</f>
-        <v>3.4578668799280003</v>
+        <f t="shared" si="15"/>
+        <v>2</v>
       </c>
       <c r="P18" s="9">
-        <f>$B$2*I9+$B$3*P17</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="R18" s="3">
-        <f t="shared" si="11"/>
-        <v>5.9579046341159447</v>
+        <f t="shared" si="17"/>
+        <v>0</v>
       </c>
       <c r="S18" s="3">
-        <f t="shared" si="12"/>
-        <v>9.210920564343251</v>
+        <f t="shared" si="18"/>
+        <v>1</v>
       </c>
       <c r="T18" s="3">
-        <f t="shared" si="13"/>
-        <v>10.987067262247361</v>
+        <f t="shared" si="19"/>
+        <v>3</v>
       </c>
       <c r="U18" s="11">
-        <f t="shared" si="14"/>
-        <v>11.956843359303004</v>
+        <f t="shared" si="20"/>
+        <v>4</v>
       </c>
       <c r="V18" s="3">
-        <f t="shared" si="15"/>
-        <v>5.9579046341159447</v>
+        <f t="shared" si="21"/>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="4:42" x14ac:dyDescent="0.2">
       <c r="D20" s="2">
         <f>$B$2*D11+$B$3*C20</f>
-        <v>2.9687290000000002</v>
+        <v>1</v>
       </c>
       <c r="E20" s="2">
-        <f t="shared" ref="E20:I20" si="17">$B$2*E11+$B$3*D20</f>
-        <v>4.5896550340000006</v>
+        <f t="shared" ref="E20:I20" si="23">$B$2*E11+$B$3*D20</f>
+        <v>1</v>
       </c>
       <c r="F20" s="2">
-        <f t="shared" si="17"/>
-        <v>5.4746806485640001</v>
+        <f t="shared" si="23"/>
+        <v>1</v>
       </c>
       <c r="G20" s="2">
-        <f t="shared" si="17"/>
-        <v>5.9579046341159447</v>
+        <f t="shared" si="23"/>
+        <v>2</v>
       </c>
       <c r="H20" s="2">
-        <f t="shared" si="17"/>
-        <v>6.221744930227306</v>
+        <f t="shared" si="23"/>
+        <v>3</v>
       </c>
       <c r="I20" s="2">
-        <f t="shared" si="17"/>
-        <v>3.3970727319041094</v>
+        <f t="shared" si="23"/>
+        <v>3</v>
       </c>
       <c r="K20" s="10">
         <f>K14+POWER($B$3,4)*0</f>
-        <v>3.4578668799280003</v>
+        <v>5</v>
       </c>
       <c r="L20" s="10">
         <f>L14+POWER($B$3,4)*L45</f>
-        <v>3.4578668799280003</v>
+        <v>4</v>
       </c>
       <c r="M20" s="10">
         <f>M14+POWER($B$3,4)*M45</f>
-        <v>3.4578668799280003</v>
+        <v>2</v>
       </c>
       <c r="N20" s="10">
         <f>N14+POWER($B$3,4)*N45</f>
-        <v>3.4578668799280003</v>
+        <v>5</v>
       </c>
       <c r="O20" s="10">
         <f>O14+POWER($B$3,4)*O45</f>
-        <v>3.4578668799280003</v>
+        <v>4</v>
       </c>
       <c r="P20" s="10">
         <f>P14+POWER($B$3,4)*P45</f>
@@ -1645,70 +1645,70 @@
       </c>
       <c r="R20" s="4">
         <f>$B$2*K20</f>
-        <v>5.9579046341159447</v>
+        <v>5</v>
       </c>
       <c r="S20" s="4">
         <f>$B$2*L20+$B$3*R20</f>
-        <v>9.210920564343251</v>
+        <v>9</v>
       </c>
       <c r="T20" s="4">
         <f>$B$2*M20+$B$3*S20</f>
-        <v>10.987067262247361</v>
+        <v>11</v>
       </c>
       <c r="U20" s="5">
         <f>$B$2*N20+$B$3*T20</f>
-        <v>11.956843359303004</v>
+        <v>16</v>
       </c>
       <c r="V20" s="4">
         <f>$B$2*O20</f>
-        <v>5.9579046341159447</v>
+        <v>4</v>
       </c>
       <c r="Z20" s="13">
         <v>1</v>
       </c>
       <c r="AA20" s="6">
         <f>U11+POWER($B$3,$Z20)*U19+POWER($B$3,4)*0</f>
-        <v>5.9579046341159447</v>
+        <v>2</v>
       </c>
       <c r="AB20" s="6">
         <f>V11+POWER($B$3,$Z20)*V19+POWER($B$3,4)*AA20</f>
-        <v>3.4982267489923817</v>
+        <v>3</v>
       </c>
       <c r="AD20" s="13" t="str">
         <f>K20 &amp; "f,"</f>
-        <v>3.457866879928f,</v>
+        <v>5f,</v>
       </c>
       <c r="AE20" s="13" t="str">
-        <f t="shared" ref="AE20:AE21" si="18">L20 &amp; "f,"</f>
-        <v>3.457866879928f,</v>
+        <f t="shared" ref="AE20:AE21" si="24">L20 &amp; "f,"</f>
+        <v>4f,</v>
       </c>
       <c r="AF20" s="13" t="str">
-        <f t="shared" ref="AF20:AF21" si="19">M20 &amp; "f,"</f>
-        <v>3.457866879928f,</v>
+        <f t="shared" ref="AF20:AF21" si="25">M20 &amp; "f,"</f>
+        <v>2f,</v>
       </c>
       <c r="AG20" s="13" t="str">
-        <f t="shared" ref="AG20:AG21" si="20">N20 &amp; "f,"</f>
-        <v>3.457866879928f,</v>
+        <f t="shared" ref="AG20:AG21" si="26">N20 &amp; "f,"</f>
+        <v>5f,</v>
       </c>
       <c r="AH20" s="13" t="str">
-        <f t="shared" ref="AH20:AH21" si="21">O20 &amp; "f,"</f>
-        <v>3.457866879928f,</v>
+        <f t="shared" ref="AH20:AH21" si="27">O20 &amp; "f,"</f>
+        <v>4f,</v>
       </c>
       <c r="AJ20" s="13" t="str">
         <f>U20 &amp; "f,"</f>
-        <v>11.956843359303f,</v>
+        <v>16f,</v>
       </c>
       <c r="AK20" s="13" t="str">
         <f>V20 &amp; "f,"</f>
-        <v>5.95790463411594f,</v>
+        <v>4f,</v>
       </c>
       <c r="AN20" s="13" t="str">
-        <f t="shared" ref="AN20:AO24" si="22">AA20 &amp; ","</f>
-        <v>5.95790463411594,</v>
+        <f t="shared" ref="AN20:AO24" si="28">AA20 &amp; ","</f>
+        <v>2,</v>
       </c>
       <c r="AO20" s="13" t="str">
-        <f t="shared" si="22"/>
-        <v>3.49822674899238,</v>
+        <f t="shared" si="28"/>
+        <v>3,</v>
       </c>
       <c r="AP20" s="1" t="e">
         <f>#REF! &amp; "f,"</f>
@@ -1717,119 +1717,119 @@
     </row>
     <row r="21" spans="4:42" x14ac:dyDescent="0.2">
       <c r="D21" s="2">
-        <f t="shared" ref="D21:I21" si="23">$B$2*D12+$B$3*C21</f>
-        <v>4.5896550340000006</v>
+        <f t="shared" ref="D21:I21" si="29">$B$2*D12+$B$3*C21</f>
+        <v>3</v>
       </c>
       <c r="E21" s="2">
-        <f t="shared" si="23"/>
-        <v>7.095606682564001</v>
+        <f t="shared" si="29"/>
+        <v>4</v>
       </c>
       <c r="F21" s="2">
-        <f t="shared" si="23"/>
-        <v>8.4638562826799451</v>
+        <f t="shared" si="29"/>
+        <v>5</v>
       </c>
       <c r="G21" s="2">
-        <f t="shared" si="23"/>
-        <v>9.210920564343251</v>
+        <f t="shared" si="29"/>
+        <v>7</v>
       </c>
       <c r="H21" s="2">
-        <f t="shared" si="23"/>
-        <v>9.6188176621314163</v>
+        <f t="shared" si="29"/>
+        <v>10</v>
       </c>
       <c r="I21" s="2">
-        <f t="shared" si="23"/>
-        <v>5.2518744435237537</v>
+        <f t="shared" si="29"/>
+        <v>10</v>
       </c>
       <c r="K21" s="10">
         <f>K18+POWER($B$3,4)*K20</f>
-        <v>3.765178399946794</v>
+        <v>5</v>
       </c>
       <c r="L21" s="10">
-        <f t="shared" ref="L21:P21" si="24">L18+POWER($B$3,4)*L20</f>
-        <v>3.765178399946794</v>
+        <f t="shared" ref="L21:P21" si="30">L18+POWER($B$3,4)*L20</f>
+        <v>5</v>
       </c>
       <c r="M21" s="10">
-        <f t="shared" si="24"/>
-        <v>3.765178399946794</v>
+        <f t="shared" si="30"/>
+        <v>4</v>
       </c>
       <c r="N21" s="10">
-        <f t="shared" si="24"/>
-        <v>3.765178399946794</v>
+        <f t="shared" si="30"/>
+        <v>6</v>
       </c>
       <c r="O21" s="10">
-        <f t="shared" si="24"/>
-        <v>3.765178399946794</v>
+        <f t="shared" si="30"/>
+        <v>6</v>
       </c>
       <c r="P21" s="10">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="R21" s="4">
-        <f t="shared" ref="R21" si="25">$B$2*K21</f>
-        <v>6.4874023831083267</v>
+        <f t="shared" ref="R21" si="31">$B$2*K21</f>
+        <v>5</v>
       </c>
       <c r="S21" s="4">
-        <f t="shared" ref="S21:U21" si="26">$B$2*L21+$B$3*R21</f>
-        <v>10.029524084285473</v>
+        <f t="shared" ref="S21:U21" si="32">$B$2*L21+$B$3*R21</f>
+        <v>10</v>
       </c>
       <c r="T21" s="4">
-        <f t="shared" si="26"/>
-        <v>11.963522533128195</v>
+        <f t="shared" si="32"/>
+        <v>14</v>
       </c>
       <c r="U21" s="5">
-        <f t="shared" si="26"/>
-        <v>13.019485686196322</v>
+        <f t="shared" si="32"/>
+        <v>20</v>
       </c>
       <c r="V21" s="4">
-        <f t="shared" ref="V21" si="27">$B$2*O21</f>
-        <v>6.4874023831083267</v>
+        <f t="shared" ref="V21" si="33">$B$2*O21</f>
+        <v>6</v>
       </c>
       <c r="Z21" s="13">
         <v>2</v>
       </c>
       <c r="AA21" s="6">
         <f>U12+POWER($B$3,Z21)*U19+POWER($B$3,4)*0</f>
-        <v>9.210920564343251</v>
+        <v>7</v>
       </c>
       <c r="AB21" s="6">
         <f>V12+POWER($B$3,$Z21)*V19+POWER($B$3,4)*AA21</f>
-        <v>5.4082585539422228</v>
+        <v>10</v>
       </c>
       <c r="AD21" s="13" t="str">
-        <f t="shared" ref="AD21" si="28">K21 &amp; "f,"</f>
-        <v>3.76517839994679f,</v>
+        <f t="shared" ref="AD21" si="34">K21 &amp; "f,"</f>
+        <v>5f,</v>
       </c>
       <c r="AE21" s="13" t="str">
-        <f t="shared" si="18"/>
-        <v>3.76517839994679f,</v>
+        <f t="shared" si="24"/>
+        <v>5f,</v>
       </c>
       <c r="AF21" s="13" t="str">
-        <f t="shared" si="19"/>
-        <v>3.76517839994679f,</v>
+        <f t="shared" si="25"/>
+        <v>4f,</v>
       </c>
       <c r="AG21" s="13" t="str">
-        <f t="shared" si="20"/>
-        <v>3.76517839994679f,</v>
+        <f t="shared" si="26"/>
+        <v>6f,</v>
       </c>
       <c r="AH21" s="13" t="str">
-        <f t="shared" si="21"/>
-        <v>3.76517839994679f,</v>
+        <f t="shared" si="27"/>
+        <v>6f,</v>
       </c>
       <c r="AJ21" s="13" t="str">
         <f>U21 &amp; "f,"</f>
-        <v>13.0194856861963f,</v>
+        <v>20f,</v>
       </c>
       <c r="AK21" s="13" t="str">
         <f>V21 &amp; "f,"</f>
-        <v>6.48740238310833f,</v>
+        <v>6f,</v>
       </c>
       <c r="AN21" s="13" t="str">
-        <f t="shared" si="22"/>
-        <v>9.21092056434325,</v>
+        <f t="shared" si="28"/>
+        <v>7,</v>
       </c>
       <c r="AO21" s="13" t="str">
-        <f t="shared" si="22"/>
-        <v>5.40825855394222,</v>
+        <f t="shared" si="28"/>
+        <v>10,</v>
       </c>
       <c r="AP21" s="1" t="e">
         <f>#REF! &amp; "f,"</f>
@@ -1838,47 +1838,47 @@
     </row>
     <row r="22" spans="4:42" x14ac:dyDescent="0.2">
       <c r="D22" s="2">
-        <f t="shared" ref="D22:I22" si="29">$B$2*D13+$B$3*C22</f>
-        <v>5.4746806485640001</v>
+        <f t="shared" ref="D22:I22" si="35">$B$2*D13+$B$3*C22</f>
+        <v>4</v>
       </c>
       <c r="E22" s="2">
-        <f t="shared" si="29"/>
-        <v>8.4638562826799451</v>
+        <f t="shared" si="35"/>
+        <v>7</v>
       </c>
       <c r="F22" s="2">
-        <f t="shared" si="29"/>
-        <v>10.095946178907251</v>
+        <f t="shared" si="35"/>
+        <v>9</v>
       </c>
       <c r="G22" s="2">
-        <f t="shared" si="29"/>
-        <v>10.98706726224736</v>
+        <f t="shared" si="35"/>
+        <v>13</v>
       </c>
       <c r="H22" s="2">
-        <f t="shared" si="29"/>
-        <v>11.47361937375106</v>
+        <f t="shared" si="35"/>
+        <v>16</v>
       </c>
       <c r="I22" s="2">
-        <f t="shared" si="29"/>
-        <v>6.2645961780680794</v>
+        <f t="shared" si="35"/>
+        <v>16</v>
       </c>
       <c r="Z22" s="13">
         <v>3</v>
       </c>
       <c r="AA22" s="6">
         <f>U13+POWER($B$3,Z22)*U19+POWER($B$3,4)*0</f>
-        <v>10.98706726224736</v>
+        <v>13</v>
       </c>
       <c r="AB22" s="6">
         <f>V13+POWER($B$3,$Z22)*V19+POWER($B$3,4)*AA22</f>
-        <v>6.4511359194448348</v>
+        <v>16</v>
       </c>
       <c r="AN22" s="13" t="str">
-        <f t="shared" si="22"/>
-        <v>10.9870672622474,</v>
+        <f t="shared" si="28"/>
+        <v>13,</v>
       </c>
       <c r="AO22" s="13" t="str">
-        <f t="shared" si="22"/>
-        <v>6.45113591944483,</v>
+        <f t="shared" si="28"/>
+        <v>16,</v>
       </c>
       <c r="AP22" s="1" t="e">
         <f>#REF! &amp; "f,"</f>
@@ -1887,47 +1887,47 @@
     </row>
     <row r="23" spans="4:42" x14ac:dyDescent="0.2">
       <c r="D23" s="2">
-        <f t="shared" ref="D23:I23" si="30">$B$2*D14+$B$3*C23</f>
-        <v>5.9579046341159447</v>
+        <f t="shared" ref="D23:I23" si="36">$B$2*D14+$B$3*C23</f>
+        <v>5</v>
       </c>
       <c r="E23" s="2">
-        <f t="shared" si="30"/>
-        <v>9.210920564343251</v>
+        <f t="shared" si="36"/>
+        <v>9</v>
       </c>
       <c r="F23" s="2">
-        <f t="shared" si="30"/>
-        <v>10.987067262247361</v>
+        <f t="shared" si="36"/>
+        <v>11</v>
       </c>
       <c r="G23" s="2">
-        <f t="shared" si="30"/>
-        <v>11.956843359303004</v>
+        <f t="shared" si="36"/>
+        <v>16</v>
       </c>
       <c r="H23" s="2">
-        <f t="shared" si="30"/>
-        <v>12.486341108295385</v>
+        <f t="shared" si="36"/>
+        <v>20</v>
       </c>
       <c r="I23" s="2">
-        <f t="shared" si="30"/>
-        <v>6.8175422451292809</v>
+        <f t="shared" si="36"/>
+        <v>20</v>
       </c>
       <c r="Z23" s="13">
         <v>4</v>
       </c>
       <c r="AA23" s="14">
         <f>U14+POWER($B$3,Z23)*U19+POWER($B$3,4)*0</f>
-        <v>11.956843359303004</v>
+        <v>16</v>
       </c>
       <c r="AB23" s="14">
         <f>V14+POWER($B$3,$Z23)*V19+POWER($B$3,4)*AA23</f>
-        <v>7.0205469610092619</v>
+        <v>20</v>
       </c>
       <c r="AN23" s="13" t="str">
-        <f t="shared" si="22"/>
-        <v>11.956843359303,</v>
+        <f t="shared" si="28"/>
+        <v>16,</v>
       </c>
       <c r="AO23" s="13" t="str">
-        <f t="shared" si="22"/>
-        <v>7.02054696100926,</v>
+        <f t="shared" si="28"/>
+        <v>20,</v>
       </c>
       <c r="AP23" s="1" t="e">
         <f>#REF! &amp; "f,"</f>
@@ -1936,114 +1936,114 @@
     </row>
     <row r="24" spans="4:42" x14ac:dyDescent="0.2">
       <c r="D24" s="2">
-        <f t="shared" ref="D24:I24" si="31">$B$2*D15+$B$3*C24</f>
-        <v>6.2217449302273069</v>
+        <f t="shared" ref="D24:I24" si="37">$B$2*D15+$B$3*C24</f>
+        <v>5</v>
       </c>
       <c r="E24" s="2">
-        <f t="shared" si="31"/>
-        <v>9.6188176621314163</v>
+        <f t="shared" si="37"/>
+        <v>10</v>
       </c>
       <c r="F24" s="2">
-        <f t="shared" si="31"/>
-        <v>11.47361937375106</v>
+        <f t="shared" si="37"/>
+        <v>14</v>
       </c>
       <c r="G24" s="2">
-        <f t="shared" si="31"/>
-        <v>12.486341108295386</v>
+        <f t="shared" si="37"/>
+        <v>20</v>
       </c>
       <c r="H24" s="2">
-        <f t="shared" si="31"/>
-        <v>13.039287175356588</v>
+        <f t="shared" si="37"/>
+        <v>26</v>
       </c>
       <c r="I24" s="2">
-        <f t="shared" si="31"/>
-        <v>7.1194507977446975</v>
+        <f t="shared" si="37"/>
+        <v>26</v>
       </c>
       <c r="J24" s="13">
         <v>1</v>
       </c>
       <c r="K24" s="2">
-        <f>K11+POWER($B$3,$J24)*K$19</f>
-        <v>1.7230000000000001</v>
+        <f t="shared" ref="K24:P27" si="38">K11+POWER($B$3,$J24)*K$19</f>
+        <v>1</v>
       </c>
       <c r="L24" s="2">
-        <f>L11+POWER($B$3,$J24)*L$19</f>
-        <v>1.7230000000000001</v>
+        <f t="shared" si="38"/>
+        <v>0</v>
       </c>
       <c r="M24" s="2">
-        <f>M11+POWER($B$3,$J24)*M$19</f>
-        <v>1.7230000000000001</v>
+        <f t="shared" si="38"/>
+        <v>0</v>
       </c>
       <c r="N24" s="2">
-        <f>N11+POWER($B$3,$J24)*N$19</f>
-        <v>1.7230000000000001</v>
+        <f t="shared" si="38"/>
+        <v>1</v>
       </c>
       <c r="O24" s="2">
-        <f>O11+POWER($B$3,$J24)*O$19</f>
-        <v>1.7230000000000001</v>
+        <f t="shared" si="38"/>
+        <v>1</v>
       </c>
       <c r="P24" s="2">
-        <f>P11+POWER($B$3,$J24)*P$19</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="R24" s="2">
         <f>$B$2*K24</f>
-        <v>2.9687290000000002</v>
+        <v>1</v>
       </c>
       <c r="S24" s="2">
         <f>$B$2*L24+$B$3*R24</f>
-        <v>4.5896550340000006</v>
+        <v>1</v>
       </c>
       <c r="T24" s="2">
         <f>$B$2*M24+$B$3*S24</f>
-        <v>5.4746806485640001</v>
+        <v>1</v>
       </c>
       <c r="U24" s="15">
         <f>$B$2*N24+$B$3*T24</f>
-        <v>5.9579046341159447</v>
+        <v>2</v>
       </c>
       <c r="V24" s="2">
-        <f>$B$2*O24+$B$3*AA20</f>
-        <v>6.221744930227306</v>
+        <f t="shared" ref="V24:V31" si="39">$B$2*O24+$B$3*AA20</f>
+        <v>3</v>
       </c>
       <c r="Z24" s="13">
         <v>1</v>
       </c>
       <c r="AA24" s="6">
         <f>U15+POWER($B$3,Z24)*U20+POWER($B$3,4)*0</f>
-        <v>12.486341108295385</v>
+        <v>20</v>
       </c>
       <c r="AB24" s="6">
         <f>V15+POWER($B$3,$Z24)*V20+POWER($B$3,4)*AA24</f>
-        <v>7.3314453897034388</v>
+        <v>26</v>
       </c>
       <c r="AD24" s="13" t="str">
         <f>R24 &amp; ","</f>
-        <v>2.968729,</v>
+        <v>1,</v>
       </c>
       <c r="AE24" s="13" t="str">
-        <f t="shared" ref="AE24:AE28" si="32">S24 &amp; ","</f>
-        <v>4.589655034,</v>
+        <f t="shared" ref="AE24:AE28" si="40">S24 &amp; ","</f>
+        <v>1,</v>
       </c>
       <c r="AF24" s="13" t="str">
-        <f t="shared" ref="AF24:AF28" si="33">T24 &amp; ","</f>
-        <v>5.474680648564,</v>
+        <f t="shared" ref="AF24:AF28" si="41">T24 &amp; ","</f>
+        <v>1,</v>
       </c>
       <c r="AG24" s="13" t="str">
-        <f t="shared" ref="AG24:AG28" si="34">U24 &amp; ","</f>
-        <v>5.95790463411594,</v>
+        <f t="shared" ref="AG24:AG28" si="42">U24 &amp; ","</f>
+        <v>2,</v>
       </c>
       <c r="AH24" s="13" t="str">
-        <f t="shared" ref="AH24:AH28" si="35">V24 &amp; ","</f>
-        <v>6.22174493022731,</v>
+        <f t="shared" ref="AH24:AH28" si="43">V24 &amp; ","</f>
+        <v>3,</v>
       </c>
       <c r="AN24" s="13" t="str">
-        <f t="shared" si="22"/>
-        <v>12.4863411082954,</v>
+        <f t="shared" si="28"/>
+        <v>20,</v>
       </c>
       <c r="AO24" s="13" t="str">
-        <f t="shared" si="22"/>
-        <v>7.33144538970344,</v>
+        <f t="shared" si="28"/>
+        <v>26,</v>
       </c>
       <c r="AP24" s="1" t="e">
         <f>#REF! &amp; "f,"</f>
@@ -2052,314 +2052,314 @@
     </row>
     <row r="25" spans="4:42" x14ac:dyDescent="0.2">
       <c r="D25" s="2">
-        <f t="shared" ref="D25:I25" si="36">$B$2*D16+$B$3*C25</f>
-        <v>6.36580173190411</v>
+        <f t="shared" ref="D25:I25" si="44">$B$2*D16+$B$3*C25</f>
+        <v>5</v>
       </c>
       <c r="E25" s="2">
-        <f t="shared" si="36"/>
-        <v>9.8415294775237534</v>
+        <f t="shared" si="44"/>
+        <v>10</v>
       </c>
       <c r="F25" s="2">
-        <f t="shared" si="36"/>
-        <v>11.739276826632079</v>
+        <f t="shared" si="44"/>
+        <v>14</v>
       </c>
       <c r="G25" s="2">
-        <f t="shared" si="36"/>
-        <v>12.775446879245226</v>
+        <f t="shared" si="44"/>
+        <v>20</v>
       </c>
       <c r="H25" s="2">
-        <f t="shared" si="36"/>
-        <v>13.341195727972003</v>
+        <f t="shared" si="44"/>
+        <v>26</v>
       </c>
       <c r="I25" s="2">
-        <f t="shared" si="36"/>
-        <v>7.2842928674727148</v>
+        <f t="shared" si="44"/>
+        <v>26</v>
       </c>
       <c r="J25" s="13">
         <v>2</v>
       </c>
       <c r="K25" s="2">
-        <f>K12+POWER($B$3,$J25)*K$19</f>
-        <v>2.6637580000000001</v>
+        <f t="shared" si="38"/>
+        <v>3</v>
       </c>
       <c r="L25" s="2">
-        <f>L12+POWER($B$3,$J25)*L$19</f>
-        <v>2.6637580000000001</v>
+        <f t="shared" si="38"/>
+        <v>1</v>
       </c>
       <c r="M25" s="2">
-        <f>M12+POWER($B$3,$J25)*M$19</f>
-        <v>2.6637580000000001</v>
+        <f t="shared" si="38"/>
+        <v>1</v>
       </c>
       <c r="N25" s="2">
-        <f>N12+POWER($B$3,$J25)*N$19</f>
-        <v>2.6637580000000001</v>
+        <f t="shared" si="38"/>
+        <v>2</v>
       </c>
       <c r="O25" s="2">
-        <f>O12+POWER($B$3,$J25)*O$19</f>
-        <v>2.6637580000000001</v>
+        <f t="shared" si="38"/>
+        <v>3</v>
       </c>
       <c r="P25" s="2">
-        <f>P12+POWER($B$3,$J25)*P$19</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="R25" s="2">
-        <f t="shared" ref="R25:R28" si="37">$B$2*K25</f>
-        <v>4.5896550340000006</v>
+        <f t="shared" ref="R25:R28" si="45">$B$2*K25</f>
+        <v>3</v>
       </c>
       <c r="S25" s="2">
-        <f t="shared" ref="S25:U25" si="38">$B$2*L25+$B$3*R25</f>
-        <v>7.095606682564001</v>
+        <f t="shared" ref="S25:U25" si="46">$B$2*L25+$B$3*R25</f>
+        <v>4</v>
       </c>
       <c r="T25" s="2">
-        <f t="shared" si="38"/>
-        <v>8.4638562826799451</v>
+        <f t="shared" si="46"/>
+        <v>5</v>
       </c>
       <c r="U25" s="15">
-        <f t="shared" si="38"/>
-        <v>9.210920564343251</v>
+        <f t="shared" si="46"/>
+        <v>7</v>
       </c>
       <c r="V25" s="2">
-        <f>$B$2*O25+$B$3*AA21</f>
-        <v>9.6188176621314163</v>
+        <f t="shared" si="39"/>
+        <v>10</v>
       </c>
       <c r="Z25" s="13">
         <v>2</v>
       </c>
       <c r="AA25" s="17">
         <f>U16+POWER($B$3,Z25)*U20+POWER($B$3,4)*0</f>
-        <v>12.775446879245226</v>
+        <v>20</v>
       </c>
       <c r="AB25" s="17">
         <f>V16+POWER($B$3,$Z25)*V23+POWER($B$3,4)*AA25</f>
-        <v>5.7250492338663506</v>
+        <v>22</v>
       </c>
       <c r="AD25" s="13" t="str">
-        <f t="shared" ref="AD25:AD28" si="39">R25 &amp; ","</f>
-        <v>4.589655034,</v>
+        <f t="shared" ref="AD25:AD28" si="47">R25 &amp; ","</f>
+        <v>3,</v>
       </c>
       <c r="AE25" s="13" t="str">
-        <f t="shared" si="32"/>
-        <v>7.095606682564,</v>
+        <f t="shared" si="40"/>
+        <v>4,</v>
       </c>
       <c r="AF25" s="13" t="str">
-        <f t="shared" si="33"/>
-        <v>8.46385628267995,</v>
+        <f t="shared" si="41"/>
+        <v>5,</v>
       </c>
       <c r="AG25" s="13" t="str">
-        <f t="shared" si="34"/>
-        <v>9.21092056434325,</v>
+        <f t="shared" si="42"/>
+        <v>7,</v>
       </c>
       <c r="AH25" s="13" t="str">
-        <f t="shared" si="35"/>
-        <v>9.61881766213142,</v>
+        <f t="shared" si="43"/>
+        <v>10,</v>
       </c>
     </row>
     <row r="26" spans="4:42" x14ac:dyDescent="0.2">
       <c r="D26" s="2">
-        <f t="shared" ref="D26:D27" si="40">$B$2*D17+$B$3*C26</f>
-        <v>6.444456745619644</v>
+        <f t="shared" ref="D26:D27" si="48">$B$2*D17+$B$3*C26</f>
+        <v>5</v>
       </c>
       <c r="E26" s="2">
-        <f t="shared" ref="E26:E27" si="41">$B$2*E17+$B$3*D26</f>
-        <v>9.9631301287279701</v>
+        <f t="shared" ref="E26:E27" si="49">$B$2*E17+$B$3*D26</f>
+        <v>10</v>
       </c>
       <c r="F26" s="2">
-        <f t="shared" ref="F26:F27" si="42">$B$2*F17+$B$3*E26</f>
-        <v>11.884325795905117</v>
+        <f t="shared" ref="F26:F27" si="50">$B$2*F17+$B$3*E26</f>
+        <v>14</v>
       </c>
       <c r="G26" s="2">
-        <f t="shared" ref="G26:G27" si="43">$B$2*G17+$B$3*F26</f>
-        <v>12.933298630183838</v>
+        <f t="shared" ref="G26:G27" si="51">$B$2*G17+$B$3*F26</f>
+        <v>20</v>
       </c>
       <c r="H26" s="2">
-        <f t="shared" ref="H26:H27" si="44">$B$2*H17+$B$3*G26</f>
-        <v>13.506037797700021</v>
+        <f t="shared" ref="H26:H27" si="52">$B$2*H17+$B$3*G26</f>
+        <v>26</v>
       </c>
       <c r="I26" s="2">
-        <f t="shared" ref="I26:I27" si="45">$B$2*I17+$B$3*H26</f>
-        <v>7.3742966375442123</v>
+        <f t="shared" ref="I26:I27" si="53">$B$2*I17+$B$3*H26</f>
+        <v>26</v>
       </c>
       <c r="J26" s="13">
         <v>3</v>
       </c>
       <c r="K26" s="2">
-        <f>K13+POWER($B$3,$J26)*K$19</f>
-        <v>3.1774118680000001</v>
+        <f t="shared" si="38"/>
+        <v>4</v>
       </c>
       <c r="L26" s="2">
-        <f>L13+POWER($B$3,$J26)*L$19</f>
-        <v>3.1774118680000001</v>
+        <f t="shared" si="38"/>
+        <v>3</v>
       </c>
       <c r="M26" s="2">
-        <f>M13+POWER($B$3,$J26)*M$19</f>
-        <v>3.1774118680000001</v>
+        <f t="shared" si="38"/>
+        <v>2</v>
       </c>
       <c r="N26" s="2">
-        <f>N13+POWER($B$3,$J26)*N$19</f>
-        <v>3.1774118680000001</v>
+        <f t="shared" si="38"/>
+        <v>4</v>
       </c>
       <c r="O26" s="2">
-        <f>O13+POWER($B$3,$J26)*O$19</f>
-        <v>3.1774118680000001</v>
+        <f t="shared" si="38"/>
+        <v>3</v>
       </c>
       <c r="P26" s="2">
-        <f>P13+POWER($B$3,$J26)*P$19</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="R26" s="2">
-        <f t="shared" si="37"/>
-        <v>5.4746806485640001</v>
+        <f t="shared" si="45"/>
+        <v>4</v>
       </c>
       <c r="S26" s="2">
-        <f t="shared" ref="S26:U26" si="46">$B$2*L26+$B$3*R26</f>
-        <v>8.4638562826799451</v>
+        <f t="shared" ref="S26:U26" si="54">$B$2*L26+$B$3*R26</f>
+        <v>7</v>
       </c>
       <c r="T26" s="2">
-        <f t="shared" si="46"/>
-        <v>10.095946178907251</v>
+        <f t="shared" si="54"/>
+        <v>9</v>
       </c>
       <c r="U26" s="15">
-        <f t="shared" si="46"/>
-        <v>10.98706726224736</v>
+        <f t="shared" si="54"/>
+        <v>13</v>
       </c>
       <c r="V26" s="2">
-        <f>$B$2*O26+$B$3*AA22</f>
-        <v>11.47361937375106</v>
+        <f t="shared" si="39"/>
+        <v>16</v>
       </c>
       <c r="Z26" s="13">
         <v>3</v>
       </c>
       <c r="AA26" s="17">
         <f>U17+POWER($B$3,Z26)*U20+POWER($B$3,4)*0</f>
-        <v>12.933298630183838</v>
+        <v>20</v>
       </c>
       <c r="AB26" s="17">
         <f>V17+POWER($B$3,$Z26)*V23+POWER($B$3,4)*AA26</f>
-        <v>6.6241036306834085</v>
+        <v>22</v>
       </c>
       <c r="AD26" s="13" t="str">
-        <f t="shared" si="39"/>
-        <v>5.474680648564,</v>
+        <f t="shared" si="47"/>
+        <v>4,</v>
       </c>
       <c r="AE26" s="13" t="str">
-        <f t="shared" si="32"/>
-        <v>8.46385628267995,</v>
+        <f t="shared" si="40"/>
+        <v>7,</v>
       </c>
       <c r="AF26" s="13" t="str">
-        <f t="shared" si="33"/>
-        <v>10.0959461789073,</v>
+        <f t="shared" si="41"/>
+        <v>9,</v>
       </c>
       <c r="AG26" s="13" t="str">
-        <f t="shared" si="34"/>
-        <v>10.9870672622474,</v>
+        <f t="shared" si="42"/>
+        <v>13,</v>
       </c>
       <c r="AH26" s="13" t="str">
-        <f t="shared" si="35"/>
-        <v>11.4736193737511,</v>
+        <f t="shared" si="43"/>
+        <v>16,</v>
       </c>
     </row>
     <row r="27" spans="4:42" x14ac:dyDescent="0.2">
       <c r="D27" s="2">
-        <f t="shared" si="40"/>
-        <v>6.4874023831083258</v>
+        <f t="shared" si="48"/>
+        <v>5</v>
       </c>
       <c r="E27" s="2">
-        <f t="shared" si="41"/>
-        <v>10.029524084285471</v>
+        <f t="shared" si="49"/>
+        <v>10</v>
       </c>
       <c r="F27" s="2">
-        <f t="shared" si="42"/>
-        <v>11.963522533128193</v>
+        <f t="shared" si="50"/>
+        <v>14</v>
       </c>
       <c r="G27" s="2">
-        <f t="shared" si="43"/>
-        <v>13.019485686196319</v>
+        <f t="shared" si="51"/>
+        <v>20</v>
       </c>
       <c r="H27" s="2">
-        <f t="shared" si="44"/>
-        <v>13.596041567771517</v>
+        <f t="shared" si="52"/>
+        <v>26</v>
       </c>
       <c r="I27" s="2">
+        <f t="shared" si="53"/>
+        <v>26</v>
+      </c>
+      <c r="J27" s="13">
+        <v>4</v>
+      </c>
+      <c r="K27" s="15">
+        <f t="shared" si="38"/>
+        <v>5</v>
+      </c>
+      <c r="L27" s="15">
+        <f t="shared" si="38"/>
+        <v>4</v>
+      </c>
+      <c r="M27" s="15">
+        <f t="shared" si="38"/>
+        <v>2</v>
+      </c>
+      <c r="N27" s="15">
+        <f t="shared" si="38"/>
+        <v>5</v>
+      </c>
+      <c r="O27" s="15">
+        <f t="shared" si="38"/>
+        <v>4</v>
+      </c>
+      <c r="P27" s="15">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="R27" s="2">
         <f t="shared" si="45"/>
-        <v>7.4234386960032488</v>
-      </c>
-      <c r="J27" s="13">
-        <v>4</v>
-      </c>
-      <c r="K27" s="15">
-        <f>K14+POWER($B$3,$J27)*K$19</f>
-        <v>3.4578668799280003</v>
-      </c>
-      <c r="L27" s="15">
-        <f>L14+POWER($B$3,$J27)*L$19</f>
-        <v>3.4578668799280003</v>
-      </c>
-      <c r="M27" s="15">
-        <f>M14+POWER($B$3,$J27)*M$19</f>
-        <v>3.4578668799280003</v>
-      </c>
-      <c r="N27" s="15">
-        <f>N14+POWER($B$3,$J27)*N$19</f>
-        <v>3.4578668799280003</v>
-      </c>
-      <c r="O27" s="15">
-        <f>O14+POWER($B$3,$J27)*O$19</f>
-        <v>3.4578668799280003</v>
-      </c>
-      <c r="P27" s="15">
-        <f>P14+POWER($B$3,$J27)*P$19</f>
-        <v>0</v>
-      </c>
-      <c r="R27" s="2">
-        <f t="shared" si="37"/>
-        <v>5.9579046341159447</v>
+        <v>5</v>
       </c>
       <c r="S27" s="2">
-        <f t="shared" ref="S27:U27" si="47">$B$2*L27+$B$3*R27</f>
-        <v>9.210920564343251</v>
+        <f t="shared" ref="S27:U27" si="55">$B$2*L27+$B$3*R27</f>
+        <v>9</v>
       </c>
       <c r="T27" s="2">
-        <f t="shared" si="47"/>
-        <v>10.987067262247361</v>
+        <f t="shared" si="55"/>
+        <v>11</v>
       </c>
       <c r="U27" s="15">
-        <f t="shared" si="47"/>
-        <v>11.956843359303004</v>
+        <f t="shared" si="55"/>
+        <v>16</v>
       </c>
       <c r="V27" s="2">
-        <f>$B$2*O27+$B$3*AA23</f>
-        <v>12.486341108295385</v>
+        <f t="shared" si="39"/>
+        <v>20</v>
       </c>
       <c r="Z27" s="13">
         <v>4</v>
       </c>
       <c r="AA27" s="18">
         <f>U18+POWER($B$3,Z27)*U20+POWER($B$3,4)*0</f>
-        <v>13.019485686196322</v>
+        <v>20</v>
       </c>
       <c r="AB27" s="18">
         <f>V18+POWER($B$3,$Z27)*V23+POWER($B$3,4)*AA27</f>
-        <v>7.1149873313455236</v>
+        <v>22</v>
       </c>
       <c r="AD27" s="13" t="str">
-        <f t="shared" si="39"/>
-        <v>5.95790463411594,</v>
+        <f t="shared" si="47"/>
+        <v>5,</v>
       </c>
       <c r="AE27" s="13" t="str">
-        <f t="shared" si="32"/>
-        <v>9.21092056434325,</v>
+        <f t="shared" si="40"/>
+        <v>9,</v>
       </c>
       <c r="AF27" s="13" t="str">
-        <f t="shared" si="33"/>
-        <v>10.9870672622474,</v>
+        <f t="shared" si="41"/>
+        <v>11,</v>
       </c>
       <c r="AG27" s="13" t="str">
-        <f t="shared" si="34"/>
-        <v>11.956843359303,</v>
+        <f t="shared" si="42"/>
+        <v>16,</v>
       </c>
       <c r="AH27" s="13" t="str">
-        <f t="shared" si="35"/>
-        <v>12.4863411082954,</v>
+        <f t="shared" si="43"/>
+        <v>20,</v>
       </c>
     </row>
     <row r="28" spans="4:42" x14ac:dyDescent="0.2">
@@ -2367,68 +2367,68 @@
         <v>1</v>
       </c>
       <c r="K28" s="2">
-        <f>K15+POWER($B$3,$J28)*K$20</f>
-        <v>3.6109953164406887</v>
+        <f t="shared" ref="K28:P28" si="56">K15+POWER($B$3,$J28)*K$20</f>
+        <v>5</v>
       </c>
       <c r="L28" s="2">
-        <f>L15+POWER($B$3,$J28)*L$20</f>
-        <v>3.6109953164406887</v>
+        <f t="shared" si="56"/>
+        <v>5</v>
       </c>
       <c r="M28" s="2">
-        <f>M15+POWER($B$3,$J28)*M$20</f>
-        <v>3.6109953164406887</v>
+        <f t="shared" si="56"/>
+        <v>4</v>
       </c>
       <c r="N28" s="2">
-        <f>N15+POWER($B$3,$J28)*N$20</f>
-        <v>3.6109953164406887</v>
+        <f t="shared" si="56"/>
+        <v>6</v>
       </c>
       <c r="O28" s="2">
-        <f>O15+POWER($B$3,$J28)*O$20</f>
-        <v>3.6109953164406887</v>
+        <f t="shared" si="56"/>
+        <v>6</v>
       </c>
       <c r="P28" s="2">
-        <f>P15+POWER($B$3,$J28)*P$20</f>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="R28" s="2">
-        <f t="shared" si="37"/>
-        <v>6.2217449302273069</v>
+        <f t="shared" si="45"/>
+        <v>5</v>
       </c>
       <c r="S28" s="2">
-        <f t="shared" ref="S28:U28" si="48">$B$2*L28+$B$3*R28</f>
-        <v>9.6188176621314163</v>
+        <f t="shared" ref="S28:U28" si="57">$B$2*L28+$B$3*R28</f>
+        <v>10</v>
       </c>
       <c r="T28" s="2">
-        <f t="shared" si="48"/>
-        <v>11.47361937375106</v>
+        <f t="shared" si="57"/>
+        <v>14</v>
       </c>
       <c r="U28" s="15">
-        <f t="shared" si="48"/>
-        <v>12.486341108295386</v>
+        <f t="shared" si="57"/>
+        <v>20</v>
       </c>
       <c r="V28" s="2">
-        <f>$B$2*O28+$B$3*AA24</f>
-        <v>13.039287175356588</v>
+        <f t="shared" si="39"/>
+        <v>26</v>
       </c>
       <c r="AD28" s="13" t="str">
-        <f t="shared" si="39"/>
-        <v>6.22174493022731,</v>
+        <f t="shared" si="47"/>
+        <v>5,</v>
       </c>
       <c r="AE28" s="13" t="str">
-        <f t="shared" si="32"/>
-        <v>9.61881766213142,</v>
+        <f t="shared" si="40"/>
+        <v>10,</v>
       </c>
       <c r="AF28" s="13" t="str">
-        <f t="shared" si="33"/>
-        <v>11.4736193737511,</v>
+        <f t="shared" si="41"/>
+        <v>14,</v>
       </c>
       <c r="AG28" s="13" t="str">
-        <f t="shared" si="34"/>
-        <v>12.4863411082954,</v>
+        <f t="shared" si="42"/>
+        <v>20,</v>
       </c>
       <c r="AH28" s="13" t="str">
-        <f t="shared" si="35"/>
-        <v>13.0392871753566,</v>
+        <f t="shared" si="43"/>
+        <v>26,</v>
       </c>
     </row>
     <row r="29" spans="4:42" x14ac:dyDescent="0.2">
@@ -2437,47 +2437,47 @@
       </c>
       <c r="K29" s="2">
         <f>K16+POWER($B$3,$J29)*K$20</f>
-        <v>3.6946034427766161</v>
+        <v>5</v>
       </c>
       <c r="L29" s="2">
-        <f t="shared" ref="L29:P29" si="49">L16+POWER($B$3,$J29)*L$20</f>
-        <v>3.6946034427766161</v>
+        <f t="shared" ref="L29:P29" si="58">L16+POWER($B$3,$J29)*L$20</f>
+        <v>5</v>
       </c>
       <c r="M29" s="2">
-        <f t="shared" si="49"/>
-        <v>3.6946034427766161</v>
+        <f t="shared" si="58"/>
+        <v>4</v>
       </c>
       <c r="N29" s="2">
-        <f t="shared" si="49"/>
-        <v>3.6946034427766161</v>
+        <f t="shared" si="58"/>
+        <v>6</v>
       </c>
       <c r="O29" s="2">
-        <f t="shared" si="49"/>
-        <v>3.6946034427766161</v>
+        <f t="shared" si="58"/>
+        <v>6</v>
       </c>
       <c r="P29" s="2">
-        <f t="shared" si="49"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="R29" s="2">
-        <f t="shared" ref="R29:R31" si="50">$B$2*K29</f>
-        <v>6.36580173190411</v>
+        <f t="shared" ref="R29:R31" si="59">$B$2*K29</f>
+        <v>5</v>
       </c>
       <c r="S29" s="2">
-        <f t="shared" ref="S29:S31" si="51">$B$2*L29+$B$3*R29</f>
-        <v>9.8415294775237534</v>
+        <f t="shared" ref="S29:S31" si="60">$B$2*L29+$B$3*R29</f>
+        <v>10</v>
       </c>
       <c r="T29" s="2">
-        <f t="shared" ref="T29:T31" si="52">$B$2*M29+$B$3*S29</f>
-        <v>11.739276826632079</v>
+        <f t="shared" ref="T29:T31" si="61">$B$2*M29+$B$3*S29</f>
+        <v>14</v>
       </c>
       <c r="U29" s="15">
-        <f t="shared" ref="U29:U31" si="53">$B$2*N29+$B$3*T29</f>
-        <v>12.775446879245226</v>
+        <f t="shared" ref="U29:U31" si="62">$B$2*N29+$B$3*T29</f>
+        <v>20</v>
       </c>
       <c r="V29" s="2">
-        <f>$B$2*O29+$B$3*AA25</f>
-        <v>13.341195727972003</v>
+        <f t="shared" si="39"/>
+        <v>26</v>
       </c>
       <c r="AD29" s="13"/>
       <c r="AE29" s="13"/>
@@ -2491,47 +2491,47 @@
       </c>
       <c r="K30" s="2">
         <f>K17+POWER($B$3,$J30)*K$20</f>
-        <v>3.7402534797560323</v>
+        <v>5</v>
       </c>
       <c r="L30" s="2">
-        <f t="shared" ref="L30:P30" si="54">L17+POWER($B$3,$J30)*L$20</f>
-        <v>3.7402534797560323</v>
+        <f t="shared" ref="L30:P30" si="63">L17+POWER($B$3,$J30)*L$20</f>
+        <v>5</v>
       </c>
       <c r="M30" s="2">
-        <f t="shared" si="54"/>
-        <v>3.7402534797560323</v>
+        <f t="shared" si="63"/>
+        <v>4</v>
       </c>
       <c r="N30" s="2">
-        <f t="shared" si="54"/>
-        <v>3.7402534797560323</v>
+        <f t="shared" si="63"/>
+        <v>6</v>
       </c>
       <c r="O30" s="2">
-        <f t="shared" si="54"/>
-        <v>3.7402534797560323</v>
+        <f t="shared" si="63"/>
+        <v>6</v>
       </c>
       <c r="P30" s="2">
-        <f t="shared" si="54"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="R30" s="2">
-        <f t="shared" si="50"/>
-        <v>6.444456745619644</v>
+        <f t="shared" si="59"/>
+        <v>5</v>
       </c>
       <c r="S30" s="2">
-        <f t="shared" si="51"/>
-        <v>9.9631301287279701</v>
+        <f t="shared" si="60"/>
+        <v>10</v>
       </c>
       <c r="T30" s="2">
-        <f t="shared" si="52"/>
-        <v>11.884325795905117</v>
+        <f t="shared" si="61"/>
+        <v>14</v>
       </c>
       <c r="U30" s="15">
-        <f t="shared" si="53"/>
-        <v>12.933298630183838</v>
+        <f t="shared" si="62"/>
+        <v>20</v>
       </c>
       <c r="V30" s="2">
-        <f>$B$2*O30+$B$3*AA26</f>
-        <v>13.506037797700021</v>
+        <f t="shared" si="39"/>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="4:42" x14ac:dyDescent="0.2">
@@ -2540,72 +2540,72 @@
       </c>
       <c r="K31" s="15">
         <f>K18+POWER($B$3,$J31)*K$20</f>
-        <v>3.765178399946794</v>
+        <v>5</v>
       </c>
       <c r="L31" s="15">
-        <f t="shared" ref="L31:P31" si="55">L18+POWER($B$3,$J31)*L$20</f>
-        <v>3.765178399946794</v>
+        <f t="shared" ref="L31:P31" si="64">L18+POWER($B$3,$J31)*L$20</f>
+        <v>5</v>
       </c>
       <c r="M31" s="15">
-        <f t="shared" si="55"/>
-        <v>3.765178399946794</v>
+        <f t="shared" si="64"/>
+        <v>4</v>
       </c>
       <c r="N31" s="15">
-        <f t="shared" si="55"/>
-        <v>3.765178399946794</v>
+        <f t="shared" si="64"/>
+        <v>6</v>
       </c>
       <c r="O31" s="15">
-        <f t="shared" si="55"/>
-        <v>3.765178399946794</v>
+        <f t="shared" si="64"/>
+        <v>6</v>
       </c>
       <c r="P31" s="15">
-        <f t="shared" si="55"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="R31" s="2">
-        <f t="shared" si="50"/>
-        <v>6.4874023831083267</v>
+        <f t="shared" si="59"/>
+        <v>5</v>
       </c>
       <c r="S31" s="2">
-        <f t="shared" si="51"/>
-        <v>10.029524084285473</v>
+        <f t="shared" si="60"/>
+        <v>10</v>
       </c>
       <c r="T31" s="2">
-        <f t="shared" si="52"/>
-        <v>11.963522533128195</v>
+        <f t="shared" si="61"/>
+        <v>14</v>
       </c>
       <c r="U31" s="15">
-        <f t="shared" si="53"/>
-        <v>13.019485686196322</v>
+        <f t="shared" si="62"/>
+        <v>20</v>
       </c>
       <c r="V31" s="2">
-        <f>$B$2*O31+$B$3*AA27</f>
-        <v>13.596041567771518</v>
+        <f t="shared" si="39"/>
+        <v>26</v>
       </c>
     </row>
     <row r="33" spans="11:22" x14ac:dyDescent="0.2">
       <c r="K33" s="7" t="str">
-        <f t="shared" ref="K33:K40" si="56">IF(ABS(K24-D11)&lt;$B$8,".","!")</f>
+        <f t="shared" ref="K33:K40" si="65">IF(ABS(K24-D11)&lt;$B$8,".","!")</f>
         <v>.</v>
       </c>
       <c r="L33" s="7" t="str">
-        <f t="shared" ref="L33:L40" si="57">IF(ABS(L24-E11)&lt;$B$8,".","!")</f>
+        <f t="shared" ref="L33:L40" si="66">IF(ABS(L24-E11)&lt;$B$8,".","!")</f>
         <v>.</v>
       </c>
       <c r="M33" s="7" t="str">
-        <f t="shared" ref="M33:M40" si="58">IF(ABS(M24-F11)&lt;$B$8,".","!")</f>
+        <f t="shared" ref="M33:M40" si="67">IF(ABS(M24-F11)&lt;$B$8,".","!")</f>
         <v>.</v>
       </c>
       <c r="N33" s="7" t="str">
-        <f t="shared" ref="N33:N40" si="59">IF(ABS(N24-G11)&lt;$B$8,".","!")</f>
+        <f t="shared" ref="N33:N40" si="68">IF(ABS(N24-G11)&lt;$B$8,".","!")</f>
         <v>.</v>
       </c>
       <c r="O33" s="7" t="str">
-        <f t="shared" ref="O33:O40" si="60">IF(ABS(O24-H11)&lt;$B$8,".","!")</f>
+        <f t="shared" ref="O33:O40" si="69">IF(ABS(O24-H11)&lt;$B$8,".","!")</f>
         <v>.</v>
       </c>
       <c r="P33" s="7" t="str">
-        <f t="shared" ref="P33:P40" si="61">IF(ABS(P24-I11)&lt;$B$8,".","!")</f>
+        <f t="shared" ref="P33:P40" si="70">IF(ABS(P24-I11)&lt;$B$8,".","!")</f>
         <v>.</v>
       </c>
       <c r="R33" s="7" t="str">
@@ -2613,341 +2613,341 @@
         <v>.</v>
       </c>
       <c r="S33" s="7" t="str">
-        <f t="shared" ref="S33:V33" si="62">IF(ABS(S24-E20)&lt;$B$8,".","!")</f>
+        <f t="shared" ref="S33:V33" si="71">IF(ABS(S24-E20)&lt;$B$8,".","!")</f>
         <v>.</v>
       </c>
       <c r="T33" s="7" t="str">
-        <f t="shared" si="62"/>
+        <f t="shared" si="71"/>
         <v>.</v>
       </c>
       <c r="U33" s="7" t="str">
-        <f t="shared" si="62"/>
+        <f t="shared" si="71"/>
         <v>.</v>
       </c>
       <c r="V33" s="7" t="str">
-        <f t="shared" si="62"/>
+        <f t="shared" si="71"/>
         <v>.</v>
       </c>
     </row>
     <row r="34" spans="11:22" x14ac:dyDescent="0.2">
       <c r="K34" s="7" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="65"/>
         <v>.</v>
       </c>
       <c r="L34" s="7" t="str">
-        <f t="shared" si="57"/>
+        <f t="shared" si="66"/>
         <v>.</v>
       </c>
       <c r="M34" s="7" t="str">
-        <f t="shared" si="58"/>
+        <f t="shared" si="67"/>
         <v>.</v>
       </c>
       <c r="N34" s="7" t="str">
-        <f t="shared" si="59"/>
+        <f t="shared" si="68"/>
         <v>.</v>
       </c>
       <c r="O34" s="7" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="69"/>
         <v>.</v>
       </c>
       <c r="P34" s="7" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="70"/>
         <v>.</v>
       </c>
       <c r="R34" s="7" t="str">
-        <f t="shared" ref="R34:V34" si="63">IF(ABS(R25-D21)&lt;$B$8,".","!")</f>
+        <f t="shared" ref="R34:V34" si="72">IF(ABS(R25-D21)&lt;$B$8,".","!")</f>
         <v>.</v>
       </c>
       <c r="S34" s="7" t="str">
-        <f t="shared" si="63"/>
+        <f t="shared" si="72"/>
         <v>.</v>
       </c>
       <c r="T34" s="7" t="str">
-        <f t="shared" si="63"/>
+        <f t="shared" si="72"/>
         <v>.</v>
       </c>
       <c r="U34" s="7" t="str">
-        <f t="shared" si="63"/>
+        <f t="shared" si="72"/>
         <v>.</v>
       </c>
       <c r="V34" s="7" t="str">
-        <f t="shared" si="63"/>
+        <f t="shared" si="72"/>
         <v>.</v>
       </c>
     </row>
     <row r="35" spans="11:22" x14ac:dyDescent="0.2">
       <c r="K35" s="7" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="65"/>
         <v>.</v>
       </c>
       <c r="L35" s="7" t="str">
-        <f t="shared" si="57"/>
+        <f t="shared" si="66"/>
         <v>.</v>
       </c>
       <c r="M35" s="7" t="str">
-        <f t="shared" si="58"/>
+        <f t="shared" si="67"/>
         <v>.</v>
       </c>
       <c r="N35" s="7" t="str">
-        <f t="shared" si="59"/>
+        <f t="shared" si="68"/>
         <v>.</v>
       </c>
       <c r="O35" s="7" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="69"/>
         <v>.</v>
       </c>
       <c r="P35" s="7" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="70"/>
         <v>.</v>
       </c>
       <c r="R35" s="7" t="str">
-        <f t="shared" ref="R35:V35" si="64">IF(ABS(R26-D22)&lt;$B$8,".","!")</f>
+        <f t="shared" ref="R35:V35" si="73">IF(ABS(R26-D22)&lt;$B$8,".","!")</f>
         <v>.</v>
       </c>
       <c r="S35" s="7" t="str">
-        <f t="shared" si="64"/>
+        <f t="shared" si="73"/>
         <v>.</v>
       </c>
       <c r="T35" s="7" t="str">
-        <f t="shared" si="64"/>
+        <f t="shared" si="73"/>
         <v>.</v>
       </c>
       <c r="U35" s="7" t="str">
-        <f t="shared" si="64"/>
+        <f t="shared" si="73"/>
         <v>.</v>
       </c>
       <c r="V35" s="7" t="str">
-        <f t="shared" si="64"/>
+        <f t="shared" si="73"/>
         <v>.</v>
       </c>
     </row>
     <row r="36" spans="11:22" x14ac:dyDescent="0.2">
       <c r="K36" s="7" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="65"/>
         <v>.</v>
       </c>
       <c r="L36" s="7" t="str">
-        <f t="shared" si="57"/>
+        <f t="shared" si="66"/>
         <v>.</v>
       </c>
       <c r="M36" s="7" t="str">
-        <f t="shared" si="58"/>
+        <f t="shared" si="67"/>
         <v>.</v>
       </c>
       <c r="N36" s="7" t="str">
-        <f t="shared" si="59"/>
+        <f t="shared" si="68"/>
         <v>.</v>
       </c>
       <c r="O36" s="7" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="69"/>
         <v>.</v>
       </c>
       <c r="P36" s="7" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="70"/>
         <v>.</v>
       </c>
       <c r="R36" s="7" t="str">
-        <f t="shared" ref="R36:V36" si="65">IF(ABS(R27-D23)&lt;$B$8,".","!")</f>
+        <f t="shared" ref="R36:V36" si="74">IF(ABS(R27-D23)&lt;$B$8,".","!")</f>
         <v>.</v>
       </c>
       <c r="S36" s="7" t="str">
-        <f t="shared" si="65"/>
+        <f t="shared" si="74"/>
         <v>.</v>
       </c>
       <c r="T36" s="7" t="str">
-        <f t="shared" si="65"/>
+        <f t="shared" si="74"/>
         <v>.</v>
       </c>
       <c r="U36" s="7" t="str">
-        <f t="shared" si="65"/>
+        <f t="shared" si="74"/>
         <v>.</v>
       </c>
       <c r="V36" s="7" t="str">
-        <f t="shared" si="65"/>
+        <f t="shared" si="74"/>
         <v>.</v>
       </c>
     </row>
     <row r="37" spans="11:22" x14ac:dyDescent="0.2">
       <c r="K37" s="7" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="65"/>
         <v>.</v>
       </c>
       <c r="L37" s="7" t="str">
-        <f t="shared" si="57"/>
+        <f t="shared" si="66"/>
         <v>.</v>
       </c>
       <c r="M37" s="7" t="str">
-        <f t="shared" si="58"/>
+        <f t="shared" si="67"/>
         <v>.</v>
       </c>
       <c r="N37" s="7" t="str">
-        <f t="shared" si="59"/>
+        <f t="shared" si="68"/>
         <v>.</v>
       </c>
       <c r="O37" s="7" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="69"/>
         <v>.</v>
       </c>
       <c r="P37" s="7" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="70"/>
         <v>.</v>
       </c>
       <c r="R37" s="7" t="str">
-        <f t="shared" ref="R37:V37" si="66">IF(ABS(R28-D24)&lt;$B$8,".","!")</f>
+        <f t="shared" ref="R37:V37" si="75">IF(ABS(R28-D24)&lt;$B$8,".","!")</f>
         <v>.</v>
       </c>
       <c r="S37" s="7" t="str">
-        <f t="shared" si="66"/>
+        <f t="shared" si="75"/>
         <v>.</v>
       </c>
       <c r="T37" s="7" t="str">
-        <f t="shared" si="66"/>
+        <f t="shared" si="75"/>
         <v>.</v>
       </c>
       <c r="U37" s="7" t="str">
-        <f t="shared" si="66"/>
+        <f t="shared" si="75"/>
         <v>.</v>
       </c>
       <c r="V37" s="7" t="str">
-        <f t="shared" si="66"/>
+        <f t="shared" si="75"/>
         <v>.</v>
       </c>
     </row>
     <row r="38" spans="11:22" x14ac:dyDescent="0.2">
       <c r="K38" s="7" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="65"/>
         <v>.</v>
       </c>
       <c r="L38" s="7" t="str">
-        <f t="shared" si="57"/>
+        <f t="shared" si="66"/>
         <v>.</v>
       </c>
       <c r="M38" s="7" t="str">
-        <f t="shared" si="58"/>
+        <f t="shared" si="67"/>
         <v>.</v>
       </c>
       <c r="N38" s="7" t="str">
-        <f t="shared" si="59"/>
+        <f t="shared" si="68"/>
         <v>.</v>
       </c>
       <c r="O38" s="7" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="69"/>
         <v>.</v>
       </c>
       <c r="P38" s="7" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="70"/>
         <v>.</v>
       </c>
       <c r="R38" s="7" t="str">
-        <f t="shared" ref="R38:V38" si="67">IF(ABS(R29-D25)&lt;$B$8,".","!")</f>
+        <f t="shared" ref="R38:V38" si="76">IF(ABS(R29-D25)&lt;$B$8,".","!")</f>
         <v>.</v>
       </c>
       <c r="S38" s="7" t="str">
-        <f t="shared" si="67"/>
+        <f t="shared" si="76"/>
         <v>.</v>
       </c>
       <c r="T38" s="7" t="str">
-        <f t="shared" si="67"/>
+        <f t="shared" si="76"/>
         <v>.</v>
       </c>
       <c r="U38" s="7" t="str">
-        <f t="shared" si="67"/>
+        <f t="shared" si="76"/>
         <v>.</v>
       </c>
       <c r="V38" s="7" t="str">
-        <f t="shared" si="67"/>
+        <f t="shared" si="76"/>
         <v>.</v>
       </c>
     </row>
     <row r="39" spans="11:22" x14ac:dyDescent="0.2">
       <c r="K39" s="7" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="65"/>
         <v>.</v>
       </c>
       <c r="L39" s="7" t="str">
-        <f t="shared" si="57"/>
+        <f t="shared" si="66"/>
         <v>.</v>
       </c>
       <c r="M39" s="7" t="str">
-        <f t="shared" si="58"/>
+        <f t="shared" si="67"/>
         <v>.</v>
       </c>
       <c r="N39" s="7" t="str">
-        <f t="shared" si="59"/>
+        <f t="shared" si="68"/>
         <v>.</v>
       </c>
       <c r="O39" s="7" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="69"/>
         <v>.</v>
       </c>
       <c r="P39" s="7" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="70"/>
         <v>.</v>
       </c>
       <c r="R39" s="7" t="str">
-        <f t="shared" ref="R39:V39" si="68">IF(ABS(R30-D26)&lt;$B$8,".","!")</f>
+        <f t="shared" ref="R39:V39" si="77">IF(ABS(R30-D26)&lt;$B$8,".","!")</f>
         <v>.</v>
       </c>
       <c r="S39" s="7" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="77"/>
         <v>.</v>
       </c>
       <c r="T39" s="7" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="77"/>
         <v>.</v>
       </c>
       <c r="U39" s="7" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="77"/>
         <v>.</v>
       </c>
       <c r="V39" s="7" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="77"/>
         <v>.</v>
       </c>
     </row>
     <row r="40" spans="11:22" x14ac:dyDescent="0.2">
       <c r="K40" s="7" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="65"/>
         <v>.</v>
       </c>
       <c r="L40" s="7" t="str">
-        <f t="shared" si="57"/>
+        <f t="shared" si="66"/>
         <v>.</v>
       </c>
       <c r="M40" s="7" t="str">
-        <f t="shared" si="58"/>
+        <f t="shared" si="67"/>
         <v>.</v>
       </c>
       <c r="N40" s="7" t="str">
-        <f t="shared" si="59"/>
+        <f t="shared" si="68"/>
         <v>.</v>
       </c>
       <c r="O40" s="7" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="69"/>
         <v>.</v>
       </c>
       <c r="P40" s="7" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="70"/>
         <v>.</v>
       </c>
       <c r="R40" s="7" t="str">
-        <f t="shared" ref="R40:V40" si="69">IF(ABS(R31-D27)&lt;$B$8,".","!")</f>
+        <f t="shared" ref="R40:V40" si="78">IF(ABS(R31-D27)&lt;$B$8,".","!")</f>
         <v>.</v>
       </c>
       <c r="S40" s="7" t="str">
-        <f t="shared" si="69"/>
+        <f t="shared" si="78"/>
         <v>.</v>
       </c>
       <c r="T40" s="7" t="str">
-        <f t="shared" si="69"/>
+        <f t="shared" si="78"/>
         <v>.</v>
       </c>
       <c r="U40" s="7" t="str">
-        <f t="shared" si="69"/>
+        <f t="shared" si="78"/>
         <v>.</v>
       </c>
       <c r="V40" s="7" t="str">
-        <f t="shared" si="69"/>
+        <f t="shared" si="78"/>
         <v>.</v>
       </c>
     </row>
@@ -3442,21 +3442,21 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
     <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3480,6 +3480,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCCBCDE3-ADC9-411E-A5F5-6F7285261F5D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{32695E15-2B13-4DDA-A339-3037F2566A9D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -3495,12 +3503,4 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCCBCDE3-ADC9-411E-A5F5-6F7285261F5D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>